<commit_message>
Fixed a typo and wrapped a line that was too long
</commit_message>
<xml_diff>
--- a/TimeReportLog(Oct2022).xlsx
+++ b/TimeReportLog(Oct2022).xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28420" windowHeight="16420" tabRatio="600" firstSheet="1" activeTab="4" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weekly Time Reporting Template" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weekly Time Reporting Oct 10." sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weekly Time Reporting Oct. 17" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weekly Time Reporting Oct 24." sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="1" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Weekly Time Reporting Dec 15." sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Weekly Time Reporting Template" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Weekly Time Reporting Oct 10." sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Weekly Time Reporting Oct. 17" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Weekly Time Reporting Oct 24." sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Weekly Time Reporting Dec 15." sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Weekly Time Reporting Dec 16." sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Weekly Time Reporting Dec 16.1" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="start_day">'1'!$AD$24</definedName>
@@ -10843,7 +10845,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName="Sheet1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
@@ -12639,16 +12641,16 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AB9" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AC9" display="CALENDAR TEMPLATES by Vertex42.com" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AD9" display="CALENDAR TEMPLATES by Vertex42.com" r:id="rId3"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AE9" display="CALENDAR TEMPLATES by Vertex42.com" r:id="rId4"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AB10" r:id="rId5"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AC10" display="https://www.vertex42.com/calendars/" r:id="rId6"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AD10" display="https://www.vertex42.com/calendars/" r:id="rId7"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="AE10" display="https://www.vertex42.com/calendars/" r:id="rId8"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K44" r:id="rId9"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="K45" r:id="rId10"/>
+    <hyperlink ref="AB9" r:id="rId1"/>
+    <hyperlink ref="AC9" display="CALENDAR TEMPLATES by Vertex42.com" r:id="rId2"/>
+    <hyperlink ref="AD9" display="CALENDAR TEMPLATES by Vertex42.com" r:id="rId3"/>
+    <hyperlink ref="AE9" display="CALENDAR TEMPLATES by Vertex42.com" r:id="rId4"/>
+    <hyperlink ref="AB10" r:id="rId5"/>
+    <hyperlink ref="AC10" display="https://www.vertex42.com/calendars/" r:id="rId6"/>
+    <hyperlink ref="AD10" display="https://www.vertex42.com/calendars/" r:id="rId7"/>
+    <hyperlink ref="AE10" display="https://www.vertex42.com/calendars/" r:id="rId8"/>
+    <hyperlink ref="K44" r:id="rId9"/>
+    <hyperlink ref="K45" r:id="rId10"/>
   </hyperlinks>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.5" right="0.5" top="0.25" bottom="0.25" header="0.25" footer="0.25"/>
@@ -14001,6 +14003,3644 @@
       </c>
       <c r="Q43" s="93" t="n">
         <v>15</v>
+      </c>
+      <c r="R43" s="94" t="n"/>
+      <c r="S43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="T43" s="100" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" s="121">
+      <c r="A44" s="155" t="inlineStr">
+        <is>
+          <t>No Additional Hours</t>
+        </is>
+      </c>
+      <c r="B44" s="126" t="n"/>
+      <c r="C44" s="95" t="n"/>
+      <c r="D44" s="68" t="n"/>
+      <c r="E44" s="155" t="n"/>
+      <c r="F44" s="126" t="n"/>
+      <c r="G44" s="95" t="n"/>
+      <c r="H44" s="147" t="n"/>
+      <c r="I44" s="156" t="n"/>
+      <c r="J44" s="126" t="n"/>
+      <c r="K44" s="95" t="n"/>
+      <c r="L44" s="95" t="n"/>
+      <c r="M44" s="156" t="n"/>
+      <c r="N44" s="126" t="n"/>
+      <c r="O44" s="95" t="n"/>
+      <c r="P44" s="95" t="n"/>
+      <c r="Q44" s="156" t="n"/>
+      <c r="R44" s="126" t="n"/>
+      <c r="S44" s="28" t="n"/>
+      <c r="T44" s="54" t="n"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1" s="121">
+      <c r="A45" s="157" t="n"/>
+      <c r="B45" s="126" t="n"/>
+      <c r="C45" s="101" t="n"/>
+      <c r="D45" s="147" t="n"/>
+      <c r="E45" s="155" t="n"/>
+      <c r="F45" s="126" t="n"/>
+      <c r="G45" s="95" t="n"/>
+      <c r="H45" s="95" t="n"/>
+      <c r="I45" s="156" t="n"/>
+      <c r="J45" s="126" t="n"/>
+      <c r="K45" s="95" t="n"/>
+      <c r="L45" s="95" t="n"/>
+      <c r="M45" s="158" t="n"/>
+      <c r="N45" s="126" t="n"/>
+      <c r="O45" s="95" t="n"/>
+      <c r="P45" s="95" t="n"/>
+      <c r="Q45" s="159" t="n"/>
+      <c r="R45" s="126" t="n"/>
+      <c r="S45" s="95" t="n"/>
+      <c r="T45" s="96" t="n"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1" s="121">
+      <c r="A46" s="157" t="n"/>
+      <c r="B46" s="126" t="n"/>
+      <c r="C46" s="101" t="n"/>
+      <c r="D46" s="95" t="n"/>
+      <c r="E46" s="159" t="n"/>
+      <c r="F46" s="126" t="n"/>
+      <c r="G46" s="95" t="n"/>
+      <c r="H46" s="95" t="n"/>
+      <c r="I46" s="156" t="n"/>
+      <c r="J46" s="126" t="n"/>
+      <c r="K46" s="95" t="n"/>
+      <c r="L46" s="95" t="n"/>
+      <c r="M46" s="151" t="n"/>
+      <c r="N46" s="126" t="n"/>
+      <c r="P46" s="95" t="n"/>
+      <c r="Q46" s="159" t="n"/>
+      <c r="R46" s="126" t="n"/>
+      <c r="S46" s="95" t="n"/>
+      <c r="T46" s="96" t="n"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1" s="121">
+      <c r="A47" s="157" t="n"/>
+      <c r="B47" s="126" t="n"/>
+      <c r="C47" s="101" t="n"/>
+      <c r="D47" s="95" t="n"/>
+      <c r="E47" s="159" t="n"/>
+      <c r="F47" s="126" t="n"/>
+      <c r="G47" s="32" t="n"/>
+      <c r="H47" s="95" t="n"/>
+      <c r="I47" s="156" t="n"/>
+      <c r="J47" s="126" t="n"/>
+      <c r="K47" s="95" t="n"/>
+      <c r="L47" s="95" t="n"/>
+      <c r="M47" s="151" t="n"/>
+      <c r="N47" s="126" t="n"/>
+      <c r="O47" s="95" t="n"/>
+      <c r="P47" s="95" t="n"/>
+      <c r="Q47" s="159" t="n"/>
+      <c r="R47" s="126" t="n"/>
+      <c r="S47" s="95" t="n"/>
+      <c r="T47" s="96" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" s="121">
+      <c r="A48" s="143" t="n"/>
+      <c r="B48" s="126" t="n"/>
+      <c r="C48" s="49" t="n"/>
+      <c r="D48" s="95" t="n"/>
+      <c r="E48" s="142" t="n"/>
+      <c r="F48" s="126" t="n"/>
+      <c r="G48" s="95" t="n"/>
+      <c r="H48" s="95" t="n"/>
+      <c r="I48" s="156" t="n"/>
+      <c r="J48" s="126" t="n"/>
+      <c r="K48" s="48" t="n"/>
+      <c r="L48" s="95" t="n"/>
+      <c r="M48" s="159" t="n"/>
+      <c r="N48" s="126" t="n"/>
+      <c r="O48" s="95" t="n"/>
+      <c r="P48" s="95" t="n"/>
+      <c r="Q48" s="165" t="n"/>
+      <c r="R48" s="126" t="n"/>
+      <c r="S48" s="95" t="n"/>
+      <c r="T48" s="96" t="n"/>
+    </row>
+    <row r="49" ht="16.5" customHeight="1" s="121">
+      <c r="A49" s="157" t="n"/>
+      <c r="B49" s="126" t="n"/>
+      <c r="C49" s="49" t="n"/>
+      <c r="D49" s="32" t="n"/>
+      <c r="E49" s="159" t="n"/>
+      <c r="F49" s="126" t="n"/>
+      <c r="G49" s="32" t="n"/>
+      <c r="H49" s="32" t="n"/>
+      <c r="I49" s="156" t="n"/>
+      <c r="J49" s="126" t="n"/>
+      <c r="K49" s="48" t="n"/>
+      <c r="L49" s="48" t="n"/>
+      <c r="M49" s="159" t="n"/>
+      <c r="N49" s="126" t="n"/>
+      <c r="O49" s="32" t="n"/>
+      <c r="P49" s="32" t="n"/>
+      <c r="Q49" s="159" t="n"/>
+      <c r="R49" s="126" t="n"/>
+      <c r="S49" s="32" t="n"/>
+      <c r="T49" s="45" t="n"/>
+    </row>
+    <row r="50" ht="13.5" customHeight="1" s="121">
+      <c r="A50" s="157" t="n"/>
+      <c r="B50" s="126" t="n"/>
+      <c r="C50" s="49" t="n"/>
+      <c r="D50" s="32" t="n"/>
+      <c r="E50" s="159" t="n"/>
+      <c r="F50" s="126" t="n"/>
+      <c r="G50" s="32" t="n"/>
+      <c r="H50" s="32" t="n"/>
+      <c r="I50" s="156" t="n"/>
+      <c r="J50" s="126" t="n"/>
+      <c r="K50" s="48" t="n"/>
+      <c r="L50" s="48" t="n"/>
+      <c r="M50" s="159" t="n"/>
+      <c r="N50" s="126" t="n"/>
+      <c r="O50" s="32" t="n"/>
+      <c r="P50" s="32" t="n"/>
+      <c r="Q50" s="159" t="n"/>
+      <c r="R50" s="126" t="n"/>
+      <c r="S50" s="32" t="n"/>
+      <c r="T50" s="45" t="n"/>
+    </row>
+    <row r="51" ht="15.75" customHeight="1" s="121">
+      <c r="A51" s="157" t="n"/>
+      <c r="B51" s="126" t="n"/>
+      <c r="C51" s="49" t="n"/>
+      <c r="D51" s="32" t="n"/>
+      <c r="E51" s="159" t="n"/>
+      <c r="F51" s="126" t="n"/>
+      <c r="G51" s="32" t="n"/>
+      <c r="H51" s="32" t="n"/>
+      <c r="I51" s="156" t="n"/>
+      <c r="J51" s="126" t="n"/>
+      <c r="K51" s="48" t="n"/>
+      <c r="L51" s="48" t="n"/>
+      <c r="M51" s="151" t="n"/>
+      <c r="N51" s="126" t="n"/>
+      <c r="O51" s="32" t="n"/>
+      <c r="P51" s="32" t="n"/>
+      <c r="Q51" s="159" t="n"/>
+      <c r="R51" s="126" t="n"/>
+      <c r="S51" s="32" t="n"/>
+      <c r="T51" s="45" t="n"/>
+    </row>
+    <row r="52" ht="16" customHeight="1" s="121">
+      <c r="A52" s="156" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="B52" s="126" t="n"/>
+      <c r="C52" s="147" t="n"/>
+      <c r="D52" s="43">
+        <f>SUM(D45:D47)</f>
+        <v/>
+      </c>
+      <c r="E52" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="F52" s="126" t="n"/>
+      <c r="G52" s="147" t="n"/>
+      <c r="H52" s="43">
+        <f>SUM(H44:H45)</f>
+        <v/>
+      </c>
+      <c r="I52" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="J52" s="126" t="n"/>
+      <c r="K52" s="147" t="n"/>
+      <c r="L52" s="43">
+        <f>SUM(L44:L47)</f>
+        <v/>
+      </c>
+      <c r="M52" s="164" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="N52" s="126" t="n"/>
+      <c r="O52" s="147" t="n"/>
+      <c r="P52" s="43">
+        <f>SUM(P44:P50)</f>
+        <v/>
+      </c>
+      <c r="Q52" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="R52" s="126" t="n"/>
+      <c r="S52" s="147" t="n"/>
+      <c r="T52" s="43">
+        <f>SUM(T47:T50)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" ht="17" customHeight="1" s="121" thickBot="1">
+      <c r="A53" s="160" t="n"/>
+      <c r="B53" s="161" t="n"/>
+      <c r="C53" s="161" t="n"/>
+      <c r="D53" s="161" t="n"/>
+      <c r="E53" s="161" t="n"/>
+      <c r="F53" s="161" t="n"/>
+      <c r="G53" s="161" t="n"/>
+      <c r="H53" s="161" t="n"/>
+      <c r="I53" s="161" t="n"/>
+      <c r="J53" s="161" t="n"/>
+      <c r="K53" s="161" t="n"/>
+      <c r="L53" s="161" t="n"/>
+      <c r="M53" s="161" t="n"/>
+      <c r="N53" s="161" t="n"/>
+      <c r="O53" s="161" t="n"/>
+      <c r="P53" s="161" t="n"/>
+      <c r="Q53" s="162" t="n"/>
+      <c r="R53" s="163" t="inlineStr">
+        <is>
+          <t>Total hours exceeded</t>
+        </is>
+      </c>
+      <c r="S53" s="162" t="n"/>
+      <c r="T53" s="66">
+        <f>SUM(D52,H52,L52,P52,T52)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="188">
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="A53:Q53"/>
+    <mergeCell ref="R53:S53"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="A41:T41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:T42"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="A33:T33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:T34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="A25:T25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:T26"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:T18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="A6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:T7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:T5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <cols>
+    <col width="11.5" customWidth="1" style="121" min="1" max="1"/>
+    <col width="10.1640625" customWidth="1" style="121" min="2" max="2"/>
+    <col width="6.83203125" customWidth="1" style="121" min="3" max="3"/>
+    <col width="8.33203125" customWidth="1" style="121" min="4" max="4"/>
+    <col width="11.5" customWidth="1" style="121" min="5" max="5"/>
+    <col width="9.83203125" customWidth="1" style="121" min="6" max="6"/>
+    <col width="6" customWidth="1" style="121" min="7" max="7"/>
+    <col width="8.1640625" customWidth="1" style="121" min="8" max="8"/>
+    <col width="11.5" customWidth="1" style="121" min="9" max="10"/>
+    <col width="7.5" customWidth="1" style="121" min="11" max="11"/>
+    <col width="7.6640625" customWidth="1" style="121" min="12" max="12"/>
+    <col width="7.33203125" customWidth="1" style="121" min="15" max="15"/>
+    <col width="7.5" customWidth="1" style="121" min="16" max="16"/>
+    <col width="6.5" customWidth="1" style="121" min="17" max="17"/>
+    <col width="15.1640625" customWidth="1" style="121" min="18" max="18"/>
+    <col width="5.6640625" customWidth="1" style="121" min="19" max="19"/>
+    <col width="8.33203125" customWidth="1" style="121" min="20" max="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1" s="121">
+      <c r="A1" s="116" t="inlineStr">
+        <is>
+          <t>Weekly Totals</t>
+        </is>
+      </c>
+      <c r="B1" s="117" t="n"/>
+      <c r="C1" s="117" t="n"/>
+      <c r="D1" s="117" t="n"/>
+      <c r="E1" s="117" t="n"/>
+      <c r="F1" s="117" t="n"/>
+      <c r="G1" s="117" t="n"/>
+      <c r="H1" s="117" t="n"/>
+      <c r="I1" s="118" t="inlineStr">
+        <is>
+          <t>Time Reporting Summery (12/12 - 12/16):</t>
+        </is>
+      </c>
+      <c r="J1" s="119" t="n"/>
+      <c r="K1" s="119" t="n"/>
+      <c r="L1" s="119" t="n"/>
+      <c r="M1" s="119" t="n"/>
+      <c r="N1" s="119" t="n"/>
+      <c r="O1" s="119" t="n"/>
+      <c r="P1" s="119" t="n"/>
+      <c r="Q1" s="119" t="n"/>
+      <c r="R1" s="119" t="n"/>
+      <c r="S1" s="119" t="n"/>
+      <c r="T1" s="120" t="n"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" s="121">
+      <c r="A2" s="125" t="n"/>
+      <c r="B2" s="126" t="n"/>
+      <c r="C2" s="84" t="inlineStr">
+        <is>
+          <t>(hrs)</t>
+        </is>
+      </c>
+      <c r="D2" s="84" t="inlineStr">
+        <is>
+          <t>% C</t>
+        </is>
+      </c>
+      <c r="E2" s="127" t="n"/>
+      <c r="F2" s="128" t="n"/>
+      <c r="G2" s="85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total </t>
+        </is>
+      </c>
+      <c r="H2" s="84" t="inlineStr">
+        <is>
+          <t>% C</t>
+        </is>
+      </c>
+      <c r="T2" s="122" t="n"/>
+    </row>
+    <row r="3" ht="19" customHeight="1" s="121">
+      <c r="A3" s="129" t="inlineStr">
+        <is>
+          <t>Overtime Paid out</t>
+        </is>
+      </c>
+      <c r="B3" s="126" t="n"/>
+      <c r="C3" s="166" t="n"/>
+      <c r="D3" s="62">
+        <f>((C3-'Weekly Time Reporting Oct 10.'!C51)/'Weekly Time Reporting Oct 10.'!C51)</f>
+        <v/>
+      </c>
+      <c r="E3" s="130" t="inlineStr">
+        <is>
+          <t>Missing Clock outs</t>
+        </is>
+      </c>
+      <c r="F3" s="126" t="n"/>
+      <c r="G3" s="65" t="n"/>
+      <c r="H3" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="122" t="n"/>
+    </row>
+    <row r="4" ht="20" customHeight="1" s="121">
+      <c r="A4" s="129" t="inlineStr">
+        <is>
+          <t>Additional Hours</t>
+        </is>
+      </c>
+      <c r="B4" s="126" t="n"/>
+      <c r="C4" s="166" t="n"/>
+      <c r="D4" s="63">
+        <f>(('Weekly Time Reporting Template'!C4-'Weekly Time Reporting Oct 10.'!C52)/'Weekly Time Reporting Oct 10.'!C52)</f>
+        <v/>
+      </c>
+      <c r="E4" s="130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Missing Clock ins </t>
+        </is>
+      </c>
+      <c r="F4" s="126" t="n"/>
+      <c r="G4" s="166" t="n"/>
+      <c r="H4" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="122" t="n"/>
+    </row>
+    <row r="5" ht="20" customHeight="1" s="121">
+      <c r="A5" s="129" t="inlineStr">
+        <is>
+          <t>Early Arrival</t>
+        </is>
+      </c>
+      <c r="B5" s="126" t="n"/>
+      <c r="C5" s="166" t="n"/>
+      <c r="D5" s="62">
+        <f>((C5-'Weekly Time Reporting Oct 10.'!C53)/'Weekly Time Reporting Oct 10.'!C53)</f>
+        <v/>
+      </c>
+      <c r="E5" s="130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absences </t>
+        </is>
+      </c>
+      <c r="F5" s="126" t="n"/>
+      <c r="G5" s="166" t="n"/>
+      <c r="H5" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="123" t="n"/>
+      <c r="J5" s="123" t="n"/>
+      <c r="K5" s="123" t="n"/>
+      <c r="L5" s="123" t="n"/>
+      <c r="M5" s="123" t="n"/>
+      <c r="N5" s="123" t="n"/>
+      <c r="O5" s="123" t="n"/>
+      <c r="P5" s="123" t="n"/>
+      <c r="Q5" s="123" t="n"/>
+      <c r="R5" s="123" t="n"/>
+      <c r="S5" s="123" t="n"/>
+      <c r="T5" s="124" t="n"/>
+    </row>
+    <row r="6" ht="27" customHeight="1" s="121">
+      <c r="A6" s="131" t="n"/>
+      <c r="B6" s="128" t="n"/>
+      <c r="C6" s="128" t="n"/>
+      <c r="D6" s="128" t="n"/>
+      <c r="E6" s="128" t="n"/>
+      <c r="F6" s="128" t="n"/>
+      <c r="G6" s="128" t="n"/>
+      <c r="H6" s="128" t="n"/>
+      <c r="I6" s="128" t="n"/>
+      <c r="J6" s="128" t="n"/>
+      <c r="K6" s="128" t="n"/>
+      <c r="L6" s="128" t="n"/>
+      <c r="M6" s="128" t="n"/>
+      <c r="N6" s="128" t="n"/>
+      <c r="O6" s="128" t="n"/>
+      <c r="P6" s="128" t="n"/>
+      <c r="Q6" s="128" t="n"/>
+      <c r="R6" s="128" t="n"/>
+      <c r="S6" s="128" t="n"/>
+      <c r="T6" s="132" t="n"/>
+    </row>
+    <row r="7" ht="45" customHeight="1" s="121">
+      <c r="A7" s="133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Early Arrivals: </t>
+        </is>
+      </c>
+      <c r="B7" s="126" t="n"/>
+      <c r="C7" s="134" t="inlineStr">
+        <is>
+          <t>Early arrivals are instances in which employees clock in prior to 8:00AM. The start time is flagged and the option is presented to managers to either round up the difference, or approve the early arrival depending on workload.</t>
+        </is>
+      </c>
+      <c r="D7" s="128" t="n"/>
+      <c r="E7" s="128" t="n"/>
+      <c r="F7" s="128" t="n"/>
+      <c r="G7" s="128" t="n"/>
+      <c r="H7" s="128" t="n"/>
+      <c r="I7" s="128" t="n"/>
+      <c r="J7" s="128" t="n"/>
+      <c r="K7" s="128" t="n"/>
+      <c r="L7" s="128" t="n"/>
+      <c r="M7" s="128" t="n"/>
+      <c r="N7" s="128" t="n"/>
+      <c r="O7" s="128" t="n"/>
+      <c r="P7" s="128" t="n"/>
+      <c r="Q7" s="128" t="n"/>
+      <c r="R7" s="128" t="n"/>
+      <c r="S7" s="128" t="n"/>
+      <c r="T7" s="132" t="n"/>
+    </row>
+    <row r="8" ht="21" customHeight="1" s="121">
+      <c r="A8" s="135" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" s="136" t="n"/>
+      <c r="C8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="D8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="E8" s="87" t="n">
+        <v>13</v>
+      </c>
+      <c r="F8" s="30" t="n"/>
+      <c r="G8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="H8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="I8" s="87" t="n">
+        <v>14</v>
+      </c>
+      <c r="J8" s="30" t="n"/>
+      <c r="K8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="L8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="M8" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N8" s="30" t="n"/>
+      <c r="O8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="P8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="Q8" s="88" t="n">
+        <v>16</v>
+      </c>
+      <c r="R8" s="30" t="n"/>
+      <c r="S8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="T8" s="176" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" s="121">
+      <c r="A9" s="137" t="inlineStr">
+        <is>
+          <t>No Early Clock ins</t>
+        </is>
+      </c>
+      <c r="B9" s="126" t="n"/>
+      <c r="C9" s="28" t="n"/>
+      <c r="D9" s="67" t="n"/>
+      <c r="E9" s="138" t="n"/>
+      <c r="F9" s="126" t="n"/>
+      <c r="G9" s="28" t="n"/>
+      <c r="H9" s="147" t="n"/>
+      <c r="I9" s="138" t="n"/>
+      <c r="J9" s="126" t="n"/>
+      <c r="K9" s="28" t="n"/>
+      <c r="L9" s="147" t="n"/>
+      <c r="M9" s="138" t="n"/>
+      <c r="N9" s="126" t="n"/>
+      <c r="O9" s="28" t="n"/>
+      <c r="P9" s="147" t="n"/>
+      <c r="Q9" s="138" t="n"/>
+      <c r="R9" s="126" t="n"/>
+      <c r="S9" s="28" t="n"/>
+      <c r="T9" s="147" t="n"/>
+    </row>
+    <row r="10" ht="16" customHeight="1" s="121">
+      <c r="A10" s="138" t="n"/>
+      <c r="B10" s="126" t="n"/>
+      <c r="C10" s="28" t="n"/>
+      <c r="D10" s="46" t="n"/>
+      <c r="E10" s="138" t="n"/>
+      <c r="F10" s="126" t="n"/>
+      <c r="G10" s="28" t="n"/>
+      <c r="H10" s="46" t="n"/>
+      <c r="I10" s="138" t="n"/>
+      <c r="J10" s="126" t="n"/>
+      <c r="K10" s="28" t="n"/>
+      <c r="L10" s="46" t="n"/>
+      <c r="M10" s="138" t="n"/>
+      <c r="N10" s="126" t="n"/>
+      <c r="O10" s="28" t="n"/>
+      <c r="P10" s="46" t="n"/>
+      <c r="Q10" s="138" t="n"/>
+      <c r="R10" s="126" t="n"/>
+      <c r="S10" s="28" t="n"/>
+      <c r="T10" s="46" t="n"/>
+    </row>
+    <row r="11" ht="16" customHeight="1" s="121">
+      <c r="A11" s="138" t="n"/>
+      <c r="B11" s="126" t="n"/>
+      <c r="C11" s="28" t="n"/>
+      <c r="D11" s="47" t="n"/>
+      <c r="E11" s="138" t="n"/>
+      <c r="F11" s="126" t="n"/>
+      <c r="G11" s="28" t="n"/>
+      <c r="H11" s="47" t="n"/>
+      <c r="I11" s="138" t="n"/>
+      <c r="J11" s="126" t="n"/>
+      <c r="K11" s="28" t="n"/>
+      <c r="L11" s="47" t="n"/>
+      <c r="M11" s="138" t="n"/>
+      <c r="N11" s="126" t="n"/>
+      <c r="O11" s="28" t="n"/>
+      <c r="P11" s="47" t="n"/>
+      <c r="Q11" s="138" t="n"/>
+      <c r="R11" s="126" t="n"/>
+      <c r="S11" s="28" t="n"/>
+      <c r="T11" s="47" t="n"/>
+    </row>
+    <row r="12" ht="16" customHeight="1" s="121">
+      <c r="A12" s="139" t="n"/>
+      <c r="B12" s="126" t="n"/>
+      <c r="C12" s="28" t="n"/>
+      <c r="D12" s="46" t="n"/>
+      <c r="E12" s="138" t="n"/>
+      <c r="F12" s="126" t="n"/>
+      <c r="G12" s="28" t="n"/>
+      <c r="H12" s="46" t="n"/>
+      <c r="I12" s="139" t="n"/>
+      <c r="J12" s="126" t="n"/>
+      <c r="K12" s="28" t="n"/>
+      <c r="L12" s="46" t="n"/>
+      <c r="M12" s="139" t="n"/>
+      <c r="N12" s="126" t="n"/>
+      <c r="O12" s="28" t="n"/>
+      <c r="P12" s="46" t="n"/>
+      <c r="Q12" s="139" t="n"/>
+      <c r="R12" s="126" t="n"/>
+      <c r="S12" s="28" t="n"/>
+      <c r="T12" s="46" t="n"/>
+    </row>
+    <row r="13" ht="16" customHeight="1" s="121">
+      <c r="A13" s="138" t="n"/>
+      <c r="B13" s="126" t="n"/>
+      <c r="C13" s="28" t="n"/>
+      <c r="D13" s="46" t="n"/>
+      <c r="E13" s="139" t="n"/>
+      <c r="F13" s="126" t="n"/>
+      <c r="G13" s="28" t="n"/>
+      <c r="H13" s="46" t="n"/>
+      <c r="I13" s="138" t="n"/>
+      <c r="J13" s="126" t="n"/>
+      <c r="K13" s="28" t="n"/>
+      <c r="L13" s="46" t="n"/>
+      <c r="M13" s="138" t="n"/>
+      <c r="N13" s="126" t="n"/>
+      <c r="O13" s="28" t="n"/>
+      <c r="P13" s="46" t="n"/>
+      <c r="Q13" s="138" t="n"/>
+      <c r="R13" s="126" t="n"/>
+      <c r="S13" s="28" t="n"/>
+      <c r="T13" s="46" t="n"/>
+    </row>
+    <row r="14" ht="16" customHeight="1" s="121">
+      <c r="A14" s="139" t="n"/>
+      <c r="B14" s="126" t="n"/>
+      <c r="C14" s="28" t="n"/>
+      <c r="D14" s="46" t="n"/>
+      <c r="E14" s="138" t="n"/>
+      <c r="F14" s="126" t="n"/>
+      <c r="G14" s="28" t="n"/>
+      <c r="H14" s="46" t="n"/>
+      <c r="I14" s="139" t="n"/>
+      <c r="J14" s="126" t="n"/>
+      <c r="K14" s="28" t="n"/>
+      <c r="L14" s="46" t="n"/>
+      <c r="M14" s="139" t="n"/>
+      <c r="N14" s="126" t="n"/>
+      <c r="O14" s="28" t="n"/>
+      <c r="P14" s="46" t="n"/>
+      <c r="Q14" s="139" t="n"/>
+      <c r="R14" s="126" t="n"/>
+      <c r="S14" s="28" t="n"/>
+      <c r="T14" s="46" t="n"/>
+    </row>
+    <row r="15" ht="16" customHeight="1" s="121">
+      <c r="A15" s="140" t="n"/>
+      <c r="B15" s="126" t="n"/>
+      <c r="C15" s="28" t="n"/>
+      <c r="D15" s="46" t="n"/>
+      <c r="E15" s="139" t="n"/>
+      <c r="F15" s="126" t="n"/>
+      <c r="G15" s="28" t="n"/>
+      <c r="H15" s="46" t="n"/>
+      <c r="I15" s="139" t="n"/>
+      <c r="J15" s="126" t="n"/>
+      <c r="K15" s="28" t="n"/>
+      <c r="L15" s="46" t="n"/>
+      <c r="M15" s="138" t="n"/>
+      <c r="N15" s="126" t="n"/>
+      <c r="O15" s="28" t="n"/>
+      <c r="P15" s="46" t="n"/>
+      <c r="Q15" s="139" t="n"/>
+      <c r="R15" s="126" t="n"/>
+      <c r="S15" s="28" t="n"/>
+      <c r="T15" s="46" t="n"/>
+    </row>
+    <row r="16" ht="16" customHeight="1" s="121">
+      <c r="A16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="B16" s="126" t="n"/>
+      <c r="C16" s="147" t="n"/>
+      <c r="D16" s="52">
+        <f>SUM(D9:D14)</f>
+        <v/>
+      </c>
+      <c r="E16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="F16" s="126" t="n"/>
+      <c r="G16" s="147" t="n"/>
+      <c r="H16" s="52">
+        <f>SUM(H9:H12)</f>
+        <v/>
+      </c>
+      <c r="I16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="J16" s="126" t="n"/>
+      <c r="K16" s="147" t="n"/>
+      <c r="L16" s="52">
+        <f>SUM(L9:L12)</f>
+        <v/>
+      </c>
+      <c r="M16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="N16" s="126" t="n"/>
+      <c r="O16" s="147" t="n"/>
+      <c r="P16" s="52">
+        <f>SUM(P9:P13)</f>
+        <v/>
+      </c>
+      <c r="Q16" s="156" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="R16" s="147" t="n"/>
+      <c r="S16" s="147" t="n"/>
+      <c r="T16" s="56">
+        <f>SUM(T9:T12)</f>
+        <v/>
+      </c>
+      <c r="U16" s="58" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="121">
+      <c r="A17" s="214" t="n"/>
+      <c r="B17" s="128" t="n"/>
+      <c r="C17" s="128" t="n"/>
+      <c r="D17" s="128" t="n"/>
+      <c r="E17" s="128" t="n"/>
+      <c r="F17" s="128" t="n"/>
+      <c r="G17" s="128" t="n"/>
+      <c r="H17" s="128" t="n"/>
+      <c r="I17" s="128" t="n"/>
+      <c r="J17" s="128" t="n"/>
+      <c r="K17" s="128" t="n"/>
+      <c r="L17" s="128" t="n"/>
+      <c r="M17" s="128" t="n"/>
+      <c r="N17" s="128" t="n"/>
+      <c r="O17" s="128" t="n"/>
+      <c r="P17" s="128" t="n"/>
+      <c r="Q17" s="126" t="n"/>
+      <c r="R17" s="145" t="inlineStr">
+        <is>
+          <t>Earnings Saved:</t>
+        </is>
+      </c>
+      <c r="S17" s="126" t="n"/>
+      <c r="T17" s="215">
+        <f>SUM(D16,H16,L16,P16,T16)*20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" ht="47" customHeight="1" s="121">
+      <c r="A18" s="141" t="inlineStr">
+        <is>
+          <t>Missing Clock Ins</t>
+        </is>
+      </c>
+      <c r="B18" s="126" t="n"/>
+      <c r="C18" s="134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Timesheets with recorded clock outs, but missing clock ins will be flagged and reported to managers. If no response is received, employees' scheduled clock in time will be manually entered. </t>
+        </is>
+      </c>
+      <c r="D18" s="128" t="n"/>
+      <c r="E18" s="128" t="n"/>
+      <c r="F18" s="128" t="n"/>
+      <c r="G18" s="128" t="n"/>
+      <c r="H18" s="128" t="n"/>
+      <c r="I18" s="128" t="n"/>
+      <c r="J18" s="128" t="n"/>
+      <c r="K18" s="128" t="n"/>
+      <c r="L18" s="128" t="n"/>
+      <c r="M18" s="128" t="n"/>
+      <c r="N18" s="128" t="n"/>
+      <c r="O18" s="128" t="n"/>
+      <c r="P18" s="128" t="n"/>
+      <c r="Q18" s="128" t="n"/>
+      <c r="R18" s="128" t="n"/>
+      <c r="S18" s="128" t="n"/>
+      <c r="T18" s="132" t="n"/>
+    </row>
+    <row r="19" ht="21" customHeight="1" s="121">
+      <c r="A19" s="91" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" s="30" t="n"/>
+      <c r="C19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="D19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="E19" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F19" s="30" t="n"/>
+      <c r="G19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="H19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="I19" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J19" s="30" t="n"/>
+      <c r="K19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="L19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="M19" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N19" s="30" t="n"/>
+      <c r="O19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="P19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="Q19" s="92" t="n">
+        <v>16</v>
+      </c>
+      <c r="R19" s="92" t="n"/>
+      <c r="S19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="T19" s="176" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="16" customHeight="1" s="121">
+      <c r="A20" s="137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No Missing Clock Ins </t>
+        </is>
+      </c>
+      <c r="B20" s="126" t="n"/>
+      <c r="C20" s="147" t="n"/>
+      <c r="D20" s="27" t="n"/>
+      <c r="E20" s="142" t="n"/>
+      <c r="F20" s="126" t="n"/>
+      <c r="G20" s="147" t="n"/>
+      <c r="H20" s="27" t="n"/>
+      <c r="I20" s="142" t="n"/>
+      <c r="J20" s="126" t="n"/>
+      <c r="K20" s="147" t="n"/>
+      <c r="L20" s="171" t="n"/>
+      <c r="M20" s="142" t="n"/>
+      <c r="N20" s="126" t="n"/>
+      <c r="O20" s="28" t="n"/>
+      <c r="P20" s="171" t="n"/>
+      <c r="Q20" s="142" t="n"/>
+      <c r="R20" s="126" t="n"/>
+      <c r="S20" s="28" t="n"/>
+      <c r="T20" s="54" t="n"/>
+    </row>
+    <row r="21" ht="16" customHeight="1" s="121">
+      <c r="A21" s="146" t="n"/>
+      <c r="B21" s="126" t="n"/>
+      <c r="C21" s="28" t="n"/>
+      <c r="D21" s="171" t="n"/>
+      <c r="E21" s="142" t="n"/>
+      <c r="F21" s="126" t="n"/>
+      <c r="G21" s="28" t="n"/>
+      <c r="H21" s="171" t="n"/>
+      <c r="I21" s="147" t="n"/>
+      <c r="J21" s="126" t="n"/>
+      <c r="K21" s="147" t="n"/>
+      <c r="L21" s="147" t="n"/>
+      <c r="M21" s="147" t="n"/>
+      <c r="N21" s="126" t="n"/>
+      <c r="O21" s="147" t="n"/>
+      <c r="P21" s="147" t="n"/>
+      <c r="Q21" s="147" t="n"/>
+      <c r="R21" s="126" t="n"/>
+      <c r="S21" s="25" t="n"/>
+      <c r="T21" s="37" t="n"/>
+    </row>
+    <row r="22" ht="16" customHeight="1" s="121">
+      <c r="A22" s="140" t="n"/>
+      <c r="B22" s="126" t="n"/>
+      <c r="C22" s="147" t="n"/>
+      <c r="D22" s="147" t="n"/>
+      <c r="E22" s="142" t="n"/>
+      <c r="F22" s="126" t="n"/>
+      <c r="G22" s="28" t="n"/>
+      <c r="H22" s="28" t="n"/>
+      <c r="I22" s="147" t="n"/>
+      <c r="J22" s="126" t="n"/>
+      <c r="K22" s="147" t="n"/>
+      <c r="L22" s="147" t="n"/>
+      <c r="M22" s="147" t="n"/>
+      <c r="N22" s="126" t="n"/>
+      <c r="O22" s="147" t="n"/>
+      <c r="P22" s="147" t="n"/>
+      <c r="Q22" s="147" t="n"/>
+      <c r="R22" s="126" t="n"/>
+      <c r="S22" s="25" t="n"/>
+      <c r="T22" s="37" t="n"/>
+    </row>
+    <row r="23" ht="16" customHeight="1" s="121">
+      <c r="A23" s="140" t="n"/>
+      <c r="B23" s="126" t="n"/>
+      <c r="C23" s="147" t="n"/>
+      <c r="D23" s="147" t="n"/>
+      <c r="E23" s="142" t="n"/>
+      <c r="F23" s="126" t="n"/>
+      <c r="G23" s="28" t="n"/>
+      <c r="H23" s="28" t="n"/>
+      <c r="I23" s="147" t="n"/>
+      <c r="J23" s="126" t="n"/>
+      <c r="K23" s="147" t="n"/>
+      <c r="L23" s="147" t="n"/>
+      <c r="M23" s="147" t="n"/>
+      <c r="N23" s="126" t="n"/>
+      <c r="O23" s="147" t="n"/>
+      <c r="P23" s="147" t="n"/>
+      <c r="Q23" s="147" t="n"/>
+      <c r="R23" s="126" t="n"/>
+      <c r="S23" s="25" t="n"/>
+      <c r="T23" s="37" t="n"/>
+    </row>
+    <row r="24" ht="16" customHeight="1" s="121">
+      <c r="A24" s="140" t="n"/>
+      <c r="B24" s="126" t="n"/>
+      <c r="C24" s="147" t="n"/>
+      <c r="D24" s="147" t="n"/>
+      <c r="E24" s="142" t="n"/>
+      <c r="F24" s="126" t="n"/>
+      <c r="G24" s="28" t="n"/>
+      <c r="H24" s="147" t="n"/>
+      <c r="I24" s="147" t="n"/>
+      <c r="J24" s="126" t="n"/>
+      <c r="K24" s="147" t="n"/>
+      <c r="L24" s="147" t="n"/>
+      <c r="M24" s="147" t="n"/>
+      <c r="N24" s="126" t="n"/>
+      <c r="O24" s="147" t="n"/>
+      <c r="P24" s="147" t="n"/>
+      <c r="Q24" s="147" t="n"/>
+      <c r="R24" s="126" t="n"/>
+      <c r="S24" s="25" t="n"/>
+      <c r="T24" s="37" t="n"/>
+    </row>
+    <row r="25" ht="17" customHeight="1" s="121">
+      <c r="A25" s="148" t="n"/>
+      <c r="B25" s="128" t="n"/>
+      <c r="C25" s="128" t="n"/>
+      <c r="D25" s="128" t="n"/>
+      <c r="E25" s="128" t="n"/>
+      <c r="F25" s="128" t="n"/>
+      <c r="G25" s="128" t="n"/>
+      <c r="H25" s="128" t="n"/>
+      <c r="I25" s="128" t="n"/>
+      <c r="J25" s="128" t="n"/>
+      <c r="K25" s="128" t="n"/>
+      <c r="L25" s="128" t="n"/>
+      <c r="M25" s="128" t="n"/>
+      <c r="N25" s="128" t="n"/>
+      <c r="O25" s="128" t="n"/>
+      <c r="P25" s="128" t="n"/>
+      <c r="Q25" s="128" t="n"/>
+      <c r="R25" s="128" t="n"/>
+      <c r="S25" s="128" t="n"/>
+      <c r="T25" s="132" t="n"/>
+    </row>
+    <row r="26" ht="44" customHeight="1" s="121">
+      <c r="A26" s="141" t="inlineStr">
+        <is>
+          <t>Missing Clock Outs</t>
+        </is>
+      </c>
+      <c r="B26" s="126" t="n"/>
+      <c r="C26" s="134" t="inlineStr">
+        <is>
+          <t>Timesheets with recorded Clock Ins but missing clock outs will be flagged and reported to managers. If no response is received, employees' scheduled clock-out  will be manually eneterd.</t>
+        </is>
+      </c>
+      <c r="D26" s="128" t="n"/>
+      <c r="E26" s="128" t="n"/>
+      <c r="F26" s="128" t="n"/>
+      <c r="G26" s="128" t="n"/>
+      <c r="H26" s="128" t="n"/>
+      <c r="I26" s="128" t="n"/>
+      <c r="J26" s="128" t="n"/>
+      <c r="K26" s="128" t="n"/>
+      <c r="L26" s="128" t="n"/>
+      <c r="M26" s="128" t="n"/>
+      <c r="N26" s="128" t="n"/>
+      <c r="O26" s="128" t="n"/>
+      <c r="P26" s="128" t="n"/>
+      <c r="Q26" s="128" t="n"/>
+      <c r="R26" s="128" t="n"/>
+      <c r="S26" s="128" t="n"/>
+      <c r="T26" s="132" t="n"/>
+    </row>
+    <row r="27" ht="21" customHeight="1" s="121">
+      <c r="A27" s="91" t="n">
+        <v>12</v>
+      </c>
+      <c r="B27" s="30" t="n"/>
+      <c r="C27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="D27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="E27" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F27" s="30" t="n"/>
+      <c r="G27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="H27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="I27" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J27" s="30" t="n"/>
+      <c r="K27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="L27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="M27" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N27" s="30" t="n"/>
+      <c r="O27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="P27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="Q27" s="93" t="n">
+        <v>16</v>
+      </c>
+      <c r="R27" s="94" t="n"/>
+      <c r="S27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="T27" s="176" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="16" customHeight="1" s="121">
+      <c r="A28" s="149" t="inlineStr">
+        <is>
+          <t>No Missing Clock Outs</t>
+        </is>
+      </c>
+      <c r="B28" s="126" t="n"/>
+      <c r="C28" s="28" t="n"/>
+      <c r="D28" s="51" t="n"/>
+      <c r="E28" s="150" t="n"/>
+      <c r="F28" s="126" t="n"/>
+      <c r="G28" s="28" t="n"/>
+      <c r="H28" s="28" t="n"/>
+      <c r="I28" s="150" t="n"/>
+      <c r="J28" s="126" t="n"/>
+      <c r="K28" s="28" t="n"/>
+      <c r="L28" s="147" t="n"/>
+      <c r="M28" s="150" t="n"/>
+      <c r="N28" s="126" t="n"/>
+      <c r="O28" s="28" t="n"/>
+      <c r="P28" s="28" t="n"/>
+      <c r="Q28" s="149" t="n"/>
+      <c r="R28" s="126" t="n"/>
+      <c r="S28" s="28" t="n"/>
+      <c r="T28" s="54" t="n"/>
+    </row>
+    <row r="29" ht="16" customHeight="1" s="121">
+      <c r="A29" s="150" t="n"/>
+      <c r="B29" s="126" t="n"/>
+      <c r="C29" s="28" t="n"/>
+      <c r="D29" s="147" t="n"/>
+      <c r="E29" s="150" t="n"/>
+      <c r="F29" s="126" t="n"/>
+      <c r="G29" s="28" t="n"/>
+      <c r="H29" s="28" t="n"/>
+      <c r="I29" s="147" t="n"/>
+      <c r="J29" s="126" t="n"/>
+      <c r="K29" s="147" t="n"/>
+      <c r="L29" s="147" t="n"/>
+      <c r="M29" s="151" t="n"/>
+      <c r="N29" s="126" t="n"/>
+      <c r="O29" s="147" t="n"/>
+      <c r="P29" s="147" t="n"/>
+      <c r="Q29" s="147" t="n"/>
+      <c r="R29" s="126" t="n"/>
+      <c r="S29" s="28" t="n"/>
+      <c r="T29" s="35" t="n"/>
+    </row>
+    <row r="30" ht="16" customHeight="1" s="121">
+      <c r="A30" s="140" t="n"/>
+      <c r="B30" s="126" t="n"/>
+      <c r="C30" s="147" t="n"/>
+      <c r="D30" s="147" t="n"/>
+      <c r="E30" s="142" t="n"/>
+      <c r="F30" s="126" t="n"/>
+      <c r="G30" s="28" t="n"/>
+      <c r="H30" s="28" t="n"/>
+      <c r="I30" s="147" t="n"/>
+      <c r="J30" s="126" t="n"/>
+      <c r="K30" s="147" t="n"/>
+      <c r="L30" s="147" t="n"/>
+      <c r="M30" s="152" t="n"/>
+      <c r="N30" s="126" t="n"/>
+      <c r="O30" s="28" t="n"/>
+      <c r="P30" s="147" t="n"/>
+      <c r="Q30" s="147" t="n"/>
+      <c r="R30" s="126" t="n"/>
+      <c r="S30" s="147" t="n"/>
+      <c r="T30" s="35" t="n"/>
+    </row>
+    <row r="31" ht="16" customHeight="1" s="121">
+      <c r="A31" s="140" t="n"/>
+      <c r="B31" s="126" t="n"/>
+      <c r="C31" s="147" t="n"/>
+      <c r="D31" s="147" t="n"/>
+      <c r="E31" s="142" t="n"/>
+      <c r="F31" s="126" t="n"/>
+      <c r="G31" s="28" t="n"/>
+      <c r="H31" s="28" t="n"/>
+      <c r="I31" s="147" t="n"/>
+      <c r="J31" s="126" t="n"/>
+      <c r="K31" s="147" t="n"/>
+      <c r="L31" s="147" t="n"/>
+      <c r="M31" s="152" t="n"/>
+      <c r="N31" s="126" t="n"/>
+      <c r="O31" s="28" t="n"/>
+      <c r="P31" s="147" t="n"/>
+      <c r="Q31" s="147" t="n"/>
+      <c r="R31" s="126" t="n"/>
+      <c r="S31" s="147" t="n"/>
+      <c r="T31" s="35" t="n"/>
+    </row>
+    <row r="32" ht="16" customHeight="1" s="121">
+      <c r="A32" s="140" t="n"/>
+      <c r="B32" s="126" t="n"/>
+      <c r="C32" s="147" t="n"/>
+      <c r="D32" s="147" t="n"/>
+      <c r="E32" s="142" t="n"/>
+      <c r="F32" s="126" t="n"/>
+      <c r="G32" s="28" t="n"/>
+      <c r="H32" s="147" t="n"/>
+      <c r="I32" s="147" t="n"/>
+      <c r="J32" s="126" t="n"/>
+      <c r="K32" s="147" t="n"/>
+      <c r="L32" s="147" t="n"/>
+      <c r="M32" s="152" t="n"/>
+      <c r="N32" s="126" t="n"/>
+      <c r="O32" s="28" t="n"/>
+      <c r="P32" s="147" t="n"/>
+      <c r="Q32" s="147" t="n"/>
+      <c r="R32" s="126" t="n"/>
+      <c r="S32" s="147" t="n"/>
+      <c r="T32" s="35" t="n"/>
+    </row>
+    <row r="33" ht="19" customHeight="1" s="121">
+      <c r="A33" s="148" t="n"/>
+      <c r="B33" s="128" t="n"/>
+      <c r="C33" s="128" t="n"/>
+      <c r="D33" s="128" t="n"/>
+      <c r="E33" s="128" t="n"/>
+      <c r="F33" s="128" t="n"/>
+      <c r="G33" s="128" t="n"/>
+      <c r="H33" s="128" t="n"/>
+      <c r="I33" s="128" t="n"/>
+      <c r="J33" s="128" t="n"/>
+      <c r="K33" s="128" t="n"/>
+      <c r="L33" s="128" t="n"/>
+      <c r="M33" s="128" t="n"/>
+      <c r="N33" s="128" t="n"/>
+      <c r="O33" s="128" t="n"/>
+      <c r="P33" s="128" t="n"/>
+      <c r="Q33" s="128" t="n"/>
+      <c r="R33" s="128" t="n"/>
+      <c r="S33" s="128" t="n"/>
+      <c r="T33" s="132" t="n"/>
+    </row>
+    <row r="34" ht="23.25" customHeight="1" s="121">
+      <c r="A34" s="133" t="inlineStr">
+        <is>
+          <t>Absences</t>
+        </is>
+      </c>
+      <c r="B34" s="126" t="n"/>
+      <c r="C34" s="153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absences will be reported to managers when an employee with a fixed schedule fails to clock in or out during their scheudled shift.  </t>
+        </is>
+      </c>
+      <c r="D34" s="128" t="n"/>
+      <c r="E34" s="128" t="n"/>
+      <c r="F34" s="128" t="n"/>
+      <c r="G34" s="128" t="n"/>
+      <c r="H34" s="128" t="n"/>
+      <c r="I34" s="128" t="n"/>
+      <c r="J34" s="128" t="n"/>
+      <c r="K34" s="128" t="n"/>
+      <c r="L34" s="128" t="n"/>
+      <c r="M34" s="128" t="n"/>
+      <c r="N34" s="128" t="n"/>
+      <c r="O34" s="128" t="n"/>
+      <c r="P34" s="128" t="n"/>
+      <c r="Q34" s="128" t="n"/>
+      <c r="R34" s="128" t="n"/>
+      <c r="S34" s="128" t="n"/>
+      <c r="T34" s="132" t="n"/>
+    </row>
+    <row r="35" ht="18.75" customHeight="1" s="121">
+      <c r="A35" s="91" t="n">
+        <v>12</v>
+      </c>
+      <c r="B35" s="30" t="n"/>
+      <c r="C35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E35" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F35" s="30" t="n"/>
+      <c r="G35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="H35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="I35" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J35" s="30" t="n"/>
+      <c r="K35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="L35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="M35" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N35" s="30" t="n"/>
+      <c r="O35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="P35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="Q35" s="93" t="n">
+        <v>16</v>
+      </c>
+      <c r="R35" s="94" t="n"/>
+      <c r="S35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="T35" s="176" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" s="121">
+      <c r="A36" s="137" t="inlineStr">
+        <is>
+          <t>No Absences</t>
+        </is>
+      </c>
+      <c r="B36" s="126" t="n"/>
+      <c r="C36" s="95" t="n"/>
+      <c r="D36" s="95" t="n"/>
+      <c r="E36" s="142" t="n"/>
+      <c r="F36" s="126" t="n"/>
+      <c r="G36" s="95" t="n"/>
+      <c r="H36" s="95" t="n"/>
+      <c r="I36" s="142" t="n"/>
+      <c r="J36" s="126" t="n"/>
+      <c r="K36" s="95" t="n"/>
+      <c r="L36" s="95" t="n"/>
+      <c r="M36" s="142" t="n"/>
+      <c r="N36" s="126" t="n"/>
+      <c r="O36" s="95" t="n"/>
+      <c r="P36" s="95" t="n"/>
+      <c r="Q36" s="142" t="n"/>
+      <c r="R36" s="126" t="n"/>
+      <c r="S36" s="95" t="n"/>
+      <c r="T36" s="96" t="n"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="121">
+      <c r="A37" s="140" t="n"/>
+      <c r="B37" s="126" t="n"/>
+      <c r="C37" s="95" t="n"/>
+      <c r="D37" s="95" t="n"/>
+      <c r="E37" s="142" t="n"/>
+      <c r="F37" s="126" t="n"/>
+      <c r="G37" s="95" t="n"/>
+      <c r="H37" s="95" t="n"/>
+      <c r="I37" s="147" t="n"/>
+      <c r="J37" s="126" t="n"/>
+      <c r="K37" s="95" t="n"/>
+      <c r="L37" s="95" t="n"/>
+      <c r="M37" s="152" t="n"/>
+      <c r="N37" s="126" t="n"/>
+      <c r="O37" s="95" t="n"/>
+      <c r="P37" s="95" t="n"/>
+      <c r="Q37" s="152" t="n"/>
+      <c r="R37" s="126" t="n"/>
+      <c r="S37" s="95" t="n"/>
+      <c r="T37" s="96" t="n"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" s="121">
+      <c r="A38" s="140" t="n"/>
+      <c r="B38" s="126" t="n"/>
+      <c r="C38" s="95" t="n"/>
+      <c r="D38" s="95" t="n"/>
+      <c r="E38" s="142" t="n"/>
+      <c r="F38" s="126" t="n"/>
+      <c r="G38" s="95" t="n"/>
+      <c r="H38" s="95" t="n"/>
+      <c r="I38" s="147" t="n"/>
+      <c r="J38" s="126" t="n"/>
+      <c r="K38" s="95" t="n"/>
+      <c r="L38" s="95" t="n"/>
+      <c r="M38" s="152" t="n"/>
+      <c r="N38" s="126" t="n"/>
+      <c r="O38" s="95" t="n"/>
+      <c r="P38" s="95" t="n"/>
+      <c r="Q38" s="152" t="n"/>
+      <c r="R38" s="126" t="n"/>
+      <c r="S38" s="95" t="n"/>
+      <c r="T38" s="96" t="n"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" s="121">
+      <c r="A39" s="140" t="n"/>
+      <c r="B39" s="126" t="n"/>
+      <c r="C39" s="95" t="n"/>
+      <c r="D39" s="95" t="n"/>
+      <c r="E39" s="142" t="n"/>
+      <c r="F39" s="126" t="n"/>
+      <c r="G39" s="95" t="n"/>
+      <c r="H39" s="95" t="n"/>
+      <c r="I39" s="147" t="n"/>
+      <c r="J39" s="126" t="n"/>
+      <c r="K39" s="95" t="n"/>
+      <c r="L39" s="95" t="n"/>
+      <c r="M39" s="152" t="n"/>
+      <c r="N39" s="126" t="n"/>
+      <c r="O39" s="95" t="n"/>
+      <c r="P39" s="95" t="n"/>
+      <c r="Q39" s="152" t="n"/>
+      <c r="R39" s="126" t="n"/>
+      <c r="S39" s="95" t="n"/>
+      <c r="T39" s="96" t="n"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" s="121">
+      <c r="A40" s="140" t="n"/>
+      <c r="B40" s="126" t="n"/>
+      <c r="C40" s="95" t="n"/>
+      <c r="D40" s="95" t="n"/>
+      <c r="E40" s="142" t="n"/>
+      <c r="F40" s="126" t="n"/>
+      <c r="G40" s="95" t="n"/>
+      <c r="H40" s="95" t="n"/>
+      <c r="I40" s="147" t="n"/>
+      <c r="J40" s="126" t="n"/>
+      <c r="K40" s="95" t="n"/>
+      <c r="L40" s="95" t="n"/>
+      <c r="M40" s="152" t="n"/>
+      <c r="N40" s="126" t="n"/>
+      <c r="O40" s="95" t="n"/>
+      <c r="P40" s="95" t="n"/>
+      <c r="Q40" s="152" t="n"/>
+      <c r="R40" s="126" t="n"/>
+      <c r="S40" s="95" t="n"/>
+      <c r="T40" s="96" t="n"/>
+    </row>
+    <row r="41" ht="17" customHeight="1" s="121">
+      <c r="A41" s="148" t="n"/>
+      <c r="B41" s="128" t="n"/>
+      <c r="C41" s="128" t="n"/>
+      <c r="D41" s="128" t="n"/>
+      <c r="E41" s="128" t="n"/>
+      <c r="F41" s="128" t="n"/>
+      <c r="G41" s="128" t="n"/>
+      <c r="H41" s="128" t="n"/>
+      <c r="I41" s="128" t="n"/>
+      <c r="J41" s="128" t="n"/>
+      <c r="K41" s="128" t="n"/>
+      <c r="L41" s="128" t="n"/>
+      <c r="M41" s="128" t="n"/>
+      <c r="N41" s="128" t="n"/>
+      <c r="O41" s="128" t="n"/>
+      <c r="P41" s="128" t="n"/>
+      <c r="Q41" s="128" t="n"/>
+      <c r="R41" s="128" t="n"/>
+      <c r="S41" s="128" t="n"/>
+      <c r="T41" s="132" t="n"/>
+    </row>
+    <row r="42" ht="43.5" customHeight="1" s="121">
+      <c r="A42" s="154" t="inlineStr">
+        <is>
+          <t>Additional Hours Worked</t>
+        </is>
+      </c>
+      <c r="B42" s="126" t="n"/>
+      <c r="C42" s="134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Timesheets with clock-outs that exceed 2+ hours of scheduled clock-out time will flagged by HomeBase and reported to managers. If no response is received, administrative action will not be taken and clock out time will be left as is. </t>
+        </is>
+      </c>
+      <c r="D42" s="128" t="n"/>
+      <c r="E42" s="128" t="n"/>
+      <c r="F42" s="128" t="n"/>
+      <c r="G42" s="128" t="n"/>
+      <c r="H42" s="128" t="n"/>
+      <c r="I42" s="128" t="n"/>
+      <c r="J42" s="128" t="n"/>
+      <c r="K42" s="128" t="n"/>
+      <c r="L42" s="128" t="n"/>
+      <c r="M42" s="128" t="n"/>
+      <c r="N42" s="128" t="n"/>
+      <c r="O42" s="128" t="n"/>
+      <c r="P42" s="128" t="n"/>
+      <c r="Q42" s="128" t="n"/>
+      <c r="R42" s="128" t="n"/>
+      <c r="S42" s="128" t="n"/>
+      <c r="T42" s="132" t="n"/>
+    </row>
+    <row r="43" ht="21" customHeight="1" s="121">
+      <c r="A43" s="97" t="n">
+        <v>12</v>
+      </c>
+      <c r="B43" s="98" t="n"/>
+      <c r="C43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="D43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="E43" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F43" s="30" t="n"/>
+      <c r="G43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="H43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="I43" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J43" s="30" t="n"/>
+      <c r="K43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="L43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="M43" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N43" s="30" t="n"/>
+      <c r="O43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="P43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="Q43" s="93" t="n">
+        <v>16</v>
+      </c>
+      <c r="R43" s="94" t="n"/>
+      <c r="S43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="T43" s="100" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1" s="121">
+      <c r="A44" s="155" t="inlineStr">
+        <is>
+          <t>No Additional Hours</t>
+        </is>
+      </c>
+      <c r="B44" s="126" t="n"/>
+      <c r="C44" s="95" t="n"/>
+      <c r="D44" s="68" t="n"/>
+      <c r="E44" s="155" t="n"/>
+      <c r="F44" s="126" t="n"/>
+      <c r="G44" s="95" t="n"/>
+      <c r="H44" s="147" t="n"/>
+      <c r="I44" s="156" t="n"/>
+      <c r="J44" s="126" t="n"/>
+      <c r="K44" s="95" t="n"/>
+      <c r="L44" s="95" t="n"/>
+      <c r="M44" s="156" t="n"/>
+      <c r="N44" s="126" t="n"/>
+      <c r="O44" s="95" t="n"/>
+      <c r="P44" s="95" t="n"/>
+      <c r="Q44" s="156" t="n"/>
+      <c r="R44" s="126" t="n"/>
+      <c r="S44" s="28" t="n"/>
+      <c r="T44" s="54" t="n"/>
+    </row>
+    <row r="45" ht="15.75" customHeight="1" s="121">
+      <c r="A45" s="157" t="n"/>
+      <c r="B45" s="126" t="n"/>
+      <c r="C45" s="101" t="n"/>
+      <c r="D45" s="147" t="n"/>
+      <c r="E45" s="155" t="n"/>
+      <c r="F45" s="126" t="n"/>
+      <c r="G45" s="95" t="n"/>
+      <c r="H45" s="95" t="n"/>
+      <c r="I45" s="156" t="n"/>
+      <c r="J45" s="126" t="n"/>
+      <c r="K45" s="95" t="n"/>
+      <c r="L45" s="95" t="n"/>
+      <c r="M45" s="158" t="n"/>
+      <c r="N45" s="126" t="n"/>
+      <c r="O45" s="95" t="n"/>
+      <c r="P45" s="95" t="n"/>
+      <c r="Q45" s="159" t="n"/>
+      <c r="R45" s="126" t="n"/>
+      <c r="S45" s="95" t="n"/>
+      <c r="T45" s="96" t="n"/>
+    </row>
+    <row r="46" ht="15.75" customHeight="1" s="121">
+      <c r="A46" s="157" t="n"/>
+      <c r="B46" s="126" t="n"/>
+      <c r="C46" s="101" t="n"/>
+      <c r="D46" s="95" t="n"/>
+      <c r="E46" s="159" t="n"/>
+      <c r="F46" s="126" t="n"/>
+      <c r="G46" s="95" t="n"/>
+      <c r="H46" s="95" t="n"/>
+      <c r="I46" s="156" t="n"/>
+      <c r="J46" s="126" t="n"/>
+      <c r="K46" s="95" t="n"/>
+      <c r="L46" s="95" t="n"/>
+      <c r="M46" s="151" t="n"/>
+      <c r="N46" s="126" t="n"/>
+      <c r="P46" s="95" t="n"/>
+      <c r="Q46" s="159" t="n"/>
+      <c r="R46" s="126" t="n"/>
+      <c r="S46" s="95" t="n"/>
+      <c r="T46" s="96" t="n"/>
+    </row>
+    <row r="47" ht="15.75" customHeight="1" s="121">
+      <c r="A47" s="157" t="n"/>
+      <c r="B47" s="126" t="n"/>
+      <c r="C47" s="101" t="n"/>
+      <c r="D47" s="95" t="n"/>
+      <c r="E47" s="159" t="n"/>
+      <c r="F47" s="126" t="n"/>
+      <c r="G47" s="32" t="n"/>
+      <c r="H47" s="95" t="n"/>
+      <c r="I47" s="156" t="n"/>
+      <c r="J47" s="126" t="n"/>
+      <c r="K47" s="95" t="n"/>
+      <c r="L47" s="95" t="n"/>
+      <c r="M47" s="151" t="n"/>
+      <c r="N47" s="126" t="n"/>
+      <c r="O47" s="95" t="n"/>
+      <c r="P47" s="95" t="n"/>
+      <c r="Q47" s="159" t="n"/>
+      <c r="R47" s="126" t="n"/>
+      <c r="S47" s="95" t="n"/>
+      <c r="T47" s="96" t="n"/>
+    </row>
+    <row r="48" ht="15.75" customHeight="1" s="121">
+      <c r="A48" s="143" t="n"/>
+      <c r="B48" s="126" t="n"/>
+      <c r="C48" s="49" t="n"/>
+      <c r="D48" s="95" t="n"/>
+      <c r="E48" s="142" t="n"/>
+      <c r="F48" s="126" t="n"/>
+      <c r="G48" s="95" t="n"/>
+      <c r="H48" s="95" t="n"/>
+      <c r="I48" s="156" t="n"/>
+      <c r="J48" s="126" t="n"/>
+      <c r="K48" s="48" t="n"/>
+      <c r="L48" s="95" t="n"/>
+      <c r="M48" s="159" t="n"/>
+      <c r="N48" s="126" t="n"/>
+      <c r="O48" s="95" t="n"/>
+      <c r="P48" s="95" t="n"/>
+      <c r="Q48" s="165" t="n"/>
+      <c r="R48" s="126" t="n"/>
+      <c r="S48" s="95" t="n"/>
+      <c r="T48" s="96" t="n"/>
+    </row>
+    <row r="49" ht="16.5" customHeight="1" s="121">
+      <c r="A49" s="157" t="n"/>
+      <c r="B49" s="126" t="n"/>
+      <c r="C49" s="49" t="n"/>
+      <c r="D49" s="32" t="n"/>
+      <c r="E49" s="159" t="n"/>
+      <c r="F49" s="126" t="n"/>
+      <c r="G49" s="32" t="n"/>
+      <c r="H49" s="32" t="n"/>
+      <c r="I49" s="156" t="n"/>
+      <c r="J49" s="126" t="n"/>
+      <c r="K49" s="48" t="n"/>
+      <c r="L49" s="48" t="n"/>
+      <c r="M49" s="159" t="n"/>
+      <c r="N49" s="126" t="n"/>
+      <c r="O49" s="32" t="n"/>
+      <c r="P49" s="32" t="n"/>
+      <c r="Q49" s="159" t="n"/>
+      <c r="R49" s="126" t="n"/>
+      <c r="S49" s="32" t="n"/>
+      <c r="T49" s="45" t="n"/>
+    </row>
+    <row r="50" ht="13.5" customHeight="1" s="121">
+      <c r="A50" s="157" t="n"/>
+      <c r="B50" s="126" t="n"/>
+      <c r="C50" s="49" t="n"/>
+      <c r="D50" s="32" t="n"/>
+      <c r="E50" s="159" t="n"/>
+      <c r="F50" s="126" t="n"/>
+      <c r="G50" s="32" t="n"/>
+      <c r="H50" s="32" t="n"/>
+      <c r="I50" s="156" t="n"/>
+      <c r="J50" s="126" t="n"/>
+      <c r="K50" s="48" t="n"/>
+      <c r="L50" s="48" t="n"/>
+      <c r="M50" s="159" t="n"/>
+      <c r="N50" s="126" t="n"/>
+      <c r="O50" s="32" t="n"/>
+      <c r="P50" s="32" t="n"/>
+      <c r="Q50" s="159" t="n"/>
+      <c r="R50" s="126" t="n"/>
+      <c r="S50" s="32" t="n"/>
+      <c r="T50" s="45" t="n"/>
+    </row>
+    <row r="51" ht="15.75" customHeight="1" s="121">
+      <c r="A51" s="157" t="n"/>
+      <c r="B51" s="126" t="n"/>
+      <c r="C51" s="49" t="n"/>
+      <c r="D51" s="32" t="n"/>
+      <c r="E51" s="159" t="n"/>
+      <c r="F51" s="126" t="n"/>
+      <c r="G51" s="32" t="n"/>
+      <c r="H51" s="32" t="n"/>
+      <c r="I51" s="156" t="n"/>
+      <c r="J51" s="126" t="n"/>
+      <c r="K51" s="48" t="n"/>
+      <c r="L51" s="48" t="n"/>
+      <c r="M51" s="151" t="n"/>
+      <c r="N51" s="126" t="n"/>
+      <c r="O51" s="32" t="n"/>
+      <c r="P51" s="32" t="n"/>
+      <c r="Q51" s="159" t="n"/>
+      <c r="R51" s="126" t="n"/>
+      <c r="S51" s="32" t="n"/>
+      <c r="T51" s="45" t="n"/>
+    </row>
+    <row r="52" ht="16" customHeight="1" s="121">
+      <c r="A52" s="156" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="B52" s="126" t="n"/>
+      <c r="C52" s="147" t="n"/>
+      <c r="D52" s="43">
+        <f>SUM(D45:D47)</f>
+        <v/>
+      </c>
+      <c r="E52" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="F52" s="126" t="n"/>
+      <c r="G52" s="147" t="n"/>
+      <c r="H52" s="43">
+        <f>SUM(H44:H45)</f>
+        <v/>
+      </c>
+      <c r="I52" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="J52" s="126" t="n"/>
+      <c r="K52" s="147" t="n"/>
+      <c r="L52" s="43">
+        <f>SUM(L44:L47)</f>
+        <v/>
+      </c>
+      <c r="M52" s="164" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="N52" s="126" t="n"/>
+      <c r="O52" s="147" t="n"/>
+      <c r="P52" s="43">
+        <f>SUM(P44:P50)</f>
+        <v/>
+      </c>
+      <c r="Q52" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="R52" s="126" t="n"/>
+      <c r="S52" s="147" t="n"/>
+      <c r="T52" s="43">
+        <f>SUM(T47:T50)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="53" ht="17" customHeight="1" s="121" thickBot="1">
+      <c r="A53" s="160" t="n"/>
+      <c r="B53" s="161" t="n"/>
+      <c r="C53" s="161" t="n"/>
+      <c r="D53" s="161" t="n"/>
+      <c r="E53" s="161" t="n"/>
+      <c r="F53" s="161" t="n"/>
+      <c r="G53" s="161" t="n"/>
+      <c r="H53" s="161" t="n"/>
+      <c r="I53" s="161" t="n"/>
+      <c r="J53" s="161" t="n"/>
+      <c r="K53" s="161" t="n"/>
+      <c r="L53" s="161" t="n"/>
+      <c r="M53" s="161" t="n"/>
+      <c r="N53" s="161" t="n"/>
+      <c r="O53" s="161" t="n"/>
+      <c r="P53" s="161" t="n"/>
+      <c r="Q53" s="162" t="n"/>
+      <c r="R53" s="163" t="inlineStr">
+        <is>
+          <t>Total hours exceeded</t>
+        </is>
+      </c>
+      <c r="S53" s="162" t="n"/>
+      <c r="T53" s="66">
+        <f>SUM(D52,H52,L52,P52,T52)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="188">
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="I50:J50"/>
+    <mergeCell ref="M50:N50"/>
+    <mergeCell ref="Q50:R50"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="I48:J48"/>
+    <mergeCell ref="M48:N48"/>
+    <mergeCell ref="Q48:R48"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="I47:J47"/>
+    <mergeCell ref="M47:N47"/>
+    <mergeCell ref="Q47:R47"/>
+    <mergeCell ref="A53:Q53"/>
+    <mergeCell ref="R53:S53"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="I51:J51"/>
+    <mergeCell ref="M51:N51"/>
+    <mergeCell ref="Q51:R51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="E52:F52"/>
+    <mergeCell ref="I52:J52"/>
+    <mergeCell ref="M52:N52"/>
+    <mergeCell ref="Q52:R52"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="I49:J49"/>
+    <mergeCell ref="M49:N49"/>
+    <mergeCell ref="Q49:R49"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="I46:J46"/>
+    <mergeCell ref="M46:N46"/>
+    <mergeCell ref="Q46:R46"/>
+    <mergeCell ref="A41:T41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="C42:T42"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="I44:J44"/>
+    <mergeCell ref="M44:N44"/>
+    <mergeCell ref="Q44:R44"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="I39:J39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="Q39:R39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="I40:J40"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="Q40:R40"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="I45:J45"/>
+    <mergeCell ref="M45:N45"/>
+    <mergeCell ref="Q45:R45"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="I37:J37"/>
+    <mergeCell ref="M37:N37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="I38:J38"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="Q38:R38"/>
+    <mergeCell ref="A33:T33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="C34:T34"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="I36:J36"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="I31:J31"/>
+    <mergeCell ref="M31:N31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="I32:J32"/>
+    <mergeCell ref="M32:N32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="M29:N29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="I30:J30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="A25:T25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:T26"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="M28:N28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="M23:N23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="M24:N24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="C18:T18"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="I20:J20"/>
+    <mergeCell ref="M20:N20"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="A17:Q17"/>
+    <mergeCell ref="R17:S17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="M10:N10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="A6:T6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C7:T7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="I1:T5"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="E5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:U53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <cols>
+    <col width="11.5" customWidth="1" style="121" min="1" max="1"/>
+    <col width="10.1640625" customWidth="1" style="121" min="2" max="2"/>
+    <col width="6.83203125" customWidth="1" style="121" min="3" max="3"/>
+    <col width="8.33203125" customWidth="1" style="121" min="4" max="4"/>
+    <col width="11.5" customWidth="1" style="121" min="5" max="5"/>
+    <col width="9.83203125" customWidth="1" style="121" min="6" max="6"/>
+    <col width="6" customWidth="1" style="121" min="7" max="7"/>
+    <col width="8.1640625" customWidth="1" style="121" min="8" max="8"/>
+    <col width="11.5" customWidth="1" style="121" min="9" max="10"/>
+    <col width="7.5" customWidth="1" style="121" min="11" max="11"/>
+    <col width="7.6640625" customWidth="1" style="121" min="12" max="12"/>
+    <col width="7.33203125" customWidth="1" style="121" min="15" max="15"/>
+    <col width="7.5" customWidth="1" style="121" min="16" max="16"/>
+    <col width="6.5" customWidth="1" style="121" min="17" max="17"/>
+    <col width="15.1640625" customWidth="1" style="121" min="18" max="18"/>
+    <col width="5.6640625" customWidth="1" style="121" min="19" max="19"/>
+    <col width="8.33203125" customWidth="1" style="121" min="20" max="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="20" customHeight="1" s="121">
+      <c r="A1" s="116" t="inlineStr">
+        <is>
+          <t>Weekly Totals</t>
+        </is>
+      </c>
+      <c r="B1" s="117" t="n"/>
+      <c r="C1" s="117" t="n"/>
+      <c r="D1" s="117" t="n"/>
+      <c r="E1" s="117" t="n"/>
+      <c r="F1" s="117" t="n"/>
+      <c r="G1" s="117" t="n"/>
+      <c r="H1" s="117" t="n"/>
+      <c r="I1" s="118" t="inlineStr">
+        <is>
+          <t>Time Reporting Summery (12/12 - 12/16):</t>
+        </is>
+      </c>
+      <c r="J1" s="119" t="n"/>
+      <c r="K1" s="119" t="n"/>
+      <c r="L1" s="119" t="n"/>
+      <c r="M1" s="119" t="n"/>
+      <c r="N1" s="119" t="n"/>
+      <c r="O1" s="119" t="n"/>
+      <c r="P1" s="119" t="n"/>
+      <c r="Q1" s="119" t="n"/>
+      <c r="R1" s="119" t="n"/>
+      <c r="S1" s="119" t="n"/>
+      <c r="T1" s="120" t="n"/>
+    </row>
+    <row r="2" ht="20" customHeight="1" s="121">
+      <c r="A2" s="125" t="n"/>
+      <c r="B2" s="126" t="n"/>
+      <c r="C2" s="84" t="inlineStr">
+        <is>
+          <t>(hrs)</t>
+        </is>
+      </c>
+      <c r="D2" s="84" t="inlineStr">
+        <is>
+          <t>% C</t>
+        </is>
+      </c>
+      <c r="E2" s="127" t="n"/>
+      <c r="F2" s="128" t="n"/>
+      <c r="G2" s="85" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total </t>
+        </is>
+      </c>
+      <c r="H2" s="84" t="inlineStr">
+        <is>
+          <t>% C</t>
+        </is>
+      </c>
+      <c r="T2" s="122" t="n"/>
+    </row>
+    <row r="3" ht="19" customHeight="1" s="121">
+      <c r="A3" s="129" t="inlineStr">
+        <is>
+          <t>Overtime Paid out</t>
+        </is>
+      </c>
+      <c r="B3" s="126" t="n"/>
+      <c r="C3" s="166" t="n"/>
+      <c r="D3" s="62">
+        <f>((C3-'Weekly Time Reporting Oct 10.'!C51)/'Weekly Time Reporting Oct 10.'!C51)</f>
+        <v/>
+      </c>
+      <c r="E3" s="130" t="inlineStr">
+        <is>
+          <t>Missing Clock outs</t>
+        </is>
+      </c>
+      <c r="F3" s="126" t="n"/>
+      <c r="G3" s="65" t="n"/>
+      <c r="H3" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T3" s="122" t="n"/>
+    </row>
+    <row r="4" ht="20" customHeight="1" s="121">
+      <c r="A4" s="129" t="inlineStr">
+        <is>
+          <t>Additional Hours</t>
+        </is>
+      </c>
+      <c r="B4" s="126" t="n"/>
+      <c r="C4" s="166" t="n"/>
+      <c r="D4" s="63">
+        <f>(('Weekly Time Reporting Template'!C4-'Weekly Time Reporting Oct 10.'!C52)/'Weekly Time Reporting Oct 10.'!C52)</f>
+        <v/>
+      </c>
+      <c r="E4" s="130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Missing Clock ins </t>
+        </is>
+      </c>
+      <c r="F4" s="126" t="n"/>
+      <c r="G4" s="166" t="n"/>
+      <c r="H4" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="T4" s="122" t="n"/>
+    </row>
+    <row r="5" ht="20" customHeight="1" s="121">
+      <c r="A5" s="129" t="inlineStr">
+        <is>
+          <t>Early Arrival</t>
+        </is>
+      </c>
+      <c r="B5" s="126" t="n"/>
+      <c r="C5" s="166" t="n"/>
+      <c r="D5" s="62">
+        <f>((C5-'Weekly Time Reporting Oct 10.'!C53)/'Weekly Time Reporting Oct 10.'!C53)</f>
+        <v/>
+      </c>
+      <c r="E5" s="130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absences </t>
+        </is>
+      </c>
+      <c r="F5" s="126" t="n"/>
+      <c r="G5" s="166" t="n"/>
+      <c r="H5" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="123" t="n"/>
+      <c r="J5" s="123" t="n"/>
+      <c r="K5" s="123" t="n"/>
+      <c r="L5" s="123" t="n"/>
+      <c r="M5" s="123" t="n"/>
+      <c r="N5" s="123" t="n"/>
+      <c r="O5" s="123" t="n"/>
+      <c r="P5" s="123" t="n"/>
+      <c r="Q5" s="123" t="n"/>
+      <c r="R5" s="123" t="n"/>
+      <c r="S5" s="123" t="n"/>
+      <c r="T5" s="124" t="n"/>
+    </row>
+    <row r="6" ht="27" customHeight="1" s="121">
+      <c r="A6" s="131" t="n"/>
+      <c r="B6" s="128" t="n"/>
+      <c r="C6" s="128" t="n"/>
+      <c r="D6" s="128" t="n"/>
+      <c r="E6" s="128" t="n"/>
+      <c r="F6" s="128" t="n"/>
+      <c r="G6" s="128" t="n"/>
+      <c r="H6" s="128" t="n"/>
+      <c r="I6" s="128" t="n"/>
+      <c r="J6" s="128" t="n"/>
+      <c r="K6" s="128" t="n"/>
+      <c r="L6" s="128" t="n"/>
+      <c r="M6" s="128" t="n"/>
+      <c r="N6" s="128" t="n"/>
+      <c r="O6" s="128" t="n"/>
+      <c r="P6" s="128" t="n"/>
+      <c r="Q6" s="128" t="n"/>
+      <c r="R6" s="128" t="n"/>
+      <c r="S6" s="128" t="n"/>
+      <c r="T6" s="132" t="n"/>
+    </row>
+    <row r="7" ht="45" customHeight="1" s="121">
+      <c r="A7" s="133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Early Arrivals: </t>
+        </is>
+      </c>
+      <c r="B7" s="126" t="n"/>
+      <c r="C7" s="134" t="inlineStr">
+        <is>
+          <t>Early arrivals are instances in which employees clock in prior to 8:00AM. The start time is flagged and the option is presented to managers to either round up the difference, or approve the early arrival depending on workload.</t>
+        </is>
+      </c>
+      <c r="D7" s="128" t="n"/>
+      <c r="E7" s="128" t="n"/>
+      <c r="F7" s="128" t="n"/>
+      <c r="G7" s="128" t="n"/>
+      <c r="H7" s="128" t="n"/>
+      <c r="I7" s="128" t="n"/>
+      <c r="J7" s="128" t="n"/>
+      <c r="K7" s="128" t="n"/>
+      <c r="L7" s="128" t="n"/>
+      <c r="M7" s="128" t="n"/>
+      <c r="N7" s="128" t="n"/>
+      <c r="O7" s="128" t="n"/>
+      <c r="P7" s="128" t="n"/>
+      <c r="Q7" s="128" t="n"/>
+      <c r="R7" s="128" t="n"/>
+      <c r="S7" s="128" t="n"/>
+      <c r="T7" s="132" t="n"/>
+    </row>
+    <row r="8" ht="21" customHeight="1" s="121">
+      <c r="A8" s="135" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" s="136" t="n"/>
+      <c r="C8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="D8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="E8" s="87" t="n">
+        <v>13</v>
+      </c>
+      <c r="F8" s="30" t="n"/>
+      <c r="G8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="H8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="I8" s="87" t="n">
+        <v>14</v>
+      </c>
+      <c r="J8" s="30" t="n"/>
+      <c r="K8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="L8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="M8" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N8" s="30" t="n"/>
+      <c r="O8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="P8" s="180" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+      <c r="Q8" s="88" t="n">
+        <v>16</v>
+      </c>
+      <c r="R8" s="30" t="n"/>
+      <c r="S8" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In </t>
+        </is>
+      </c>
+      <c r="T8" s="176" t="inlineStr">
+        <is>
+          <t>hrs</t>
+        </is>
+      </c>
+    </row>
+    <row r="9" ht="16" customHeight="1" s="121">
+      <c r="A9" s="137" t="inlineStr">
+        <is>
+          <t>No Early Clock ins</t>
+        </is>
+      </c>
+      <c r="B9" s="126" t="n"/>
+      <c r="C9" s="28" t="n"/>
+      <c r="D9" s="67" t="n"/>
+      <c r="E9" s="138" t="n"/>
+      <c r="F9" s="126" t="n"/>
+      <c r="G9" s="28" t="n"/>
+      <c r="H9" s="147" t="n"/>
+      <c r="I9" s="138" t="n"/>
+      <c r="J9" s="126" t="n"/>
+      <c r="K9" s="28" t="n"/>
+      <c r="L9" s="147" t="n"/>
+      <c r="M9" s="138" t="n"/>
+      <c r="N9" s="126" t="n"/>
+      <c r="O9" s="28" t="n"/>
+      <c r="P9" s="147" t="n"/>
+      <c r="Q9" s="138" t="n"/>
+      <c r="R9" s="126" t="n"/>
+      <c r="S9" s="28" t="n"/>
+      <c r="T9" s="147" t="n"/>
+    </row>
+    <row r="10" ht="16" customHeight="1" s="121">
+      <c r="A10" s="138" t="n"/>
+      <c r="B10" s="126" t="n"/>
+      <c r="C10" s="28" t="n"/>
+      <c r="D10" s="46" t="n"/>
+      <c r="E10" s="138" t="n"/>
+      <c r="F10" s="126" t="n"/>
+      <c r="G10" s="28" t="n"/>
+      <c r="H10" s="46" t="n"/>
+      <c r="I10" s="138" t="n"/>
+      <c r="J10" s="126" t="n"/>
+      <c r="K10" s="28" t="n"/>
+      <c r="L10" s="46" t="n"/>
+      <c r="M10" s="138" t="n"/>
+      <c r="N10" s="126" t="n"/>
+      <c r="O10" s="28" t="n"/>
+      <c r="P10" s="46" t="n"/>
+      <c r="Q10" s="138" t="n"/>
+      <c r="R10" s="126" t="n"/>
+      <c r="S10" s="28" t="n"/>
+      <c r="T10" s="46" t="n"/>
+    </row>
+    <row r="11" ht="16" customHeight="1" s="121">
+      <c r="A11" s="138" t="n"/>
+      <c r="B11" s="126" t="n"/>
+      <c r="C11" s="28" t="n"/>
+      <c r="D11" s="47" t="n"/>
+      <c r="E11" s="138" t="n"/>
+      <c r="F11" s="126" t="n"/>
+      <c r="G11" s="28" t="n"/>
+      <c r="H11" s="47" t="n"/>
+      <c r="I11" s="138" t="n"/>
+      <c r="J11" s="126" t="n"/>
+      <c r="K11" s="28" t="n"/>
+      <c r="L11" s="47" t="n"/>
+      <c r="M11" s="138" t="n"/>
+      <c r="N11" s="126" t="n"/>
+      <c r="O11" s="28" t="n"/>
+      <c r="P11" s="47" t="n"/>
+      <c r="Q11" s="138" t="n"/>
+      <c r="R11" s="126" t="n"/>
+      <c r="S11" s="28" t="n"/>
+      <c r="T11" s="47" t="n"/>
+    </row>
+    <row r="12" ht="16" customHeight="1" s="121">
+      <c r="A12" s="139" t="n"/>
+      <c r="B12" s="126" t="n"/>
+      <c r="C12" s="28" t="n"/>
+      <c r="D12" s="46" t="n"/>
+      <c r="E12" s="138" t="n"/>
+      <c r="F12" s="126" t="n"/>
+      <c r="G12" s="28" t="n"/>
+      <c r="H12" s="46" t="n"/>
+      <c r="I12" s="139" t="n"/>
+      <c r="J12" s="126" t="n"/>
+      <c r="K12" s="28" t="n"/>
+      <c r="L12" s="46" t="n"/>
+      <c r="M12" s="139" t="n"/>
+      <c r="N12" s="126" t="n"/>
+      <c r="O12" s="28" t="n"/>
+      <c r="P12" s="46" t="n"/>
+      <c r="Q12" s="139" t="n"/>
+      <c r="R12" s="126" t="n"/>
+      <c r="S12" s="28" t="n"/>
+      <c r="T12" s="46" t="n"/>
+    </row>
+    <row r="13" ht="16" customHeight="1" s="121">
+      <c r="A13" s="138" t="n"/>
+      <c r="B13" s="126" t="n"/>
+      <c r="C13" s="28" t="n"/>
+      <c r="D13" s="46" t="n"/>
+      <c r="E13" s="139" t="n"/>
+      <c r="F13" s="126" t="n"/>
+      <c r="G13" s="28" t="n"/>
+      <c r="H13" s="46" t="n"/>
+      <c r="I13" s="138" t="n"/>
+      <c r="J13" s="126" t="n"/>
+      <c r="K13" s="28" t="n"/>
+      <c r="L13" s="46" t="n"/>
+      <c r="M13" s="138" t="n"/>
+      <c r="N13" s="126" t="n"/>
+      <c r="O13" s="28" t="n"/>
+      <c r="P13" s="46" t="n"/>
+      <c r="Q13" s="138" t="n"/>
+      <c r="R13" s="126" t="n"/>
+      <c r="S13" s="28" t="n"/>
+      <c r="T13" s="46" t="n"/>
+    </row>
+    <row r="14" ht="16" customHeight="1" s="121">
+      <c r="A14" s="139" t="n"/>
+      <c r="B14" s="126" t="n"/>
+      <c r="C14" s="28" t="n"/>
+      <c r="D14" s="46" t="n"/>
+      <c r="E14" s="138" t="n"/>
+      <c r="F14" s="126" t="n"/>
+      <c r="G14" s="28" t="n"/>
+      <c r="H14" s="46" t="n"/>
+      <c r="I14" s="139" t="n"/>
+      <c r="J14" s="126" t="n"/>
+      <c r="K14" s="28" t="n"/>
+      <c r="L14" s="46" t="n"/>
+      <c r="M14" s="139" t="n"/>
+      <c r="N14" s="126" t="n"/>
+      <c r="O14" s="28" t="n"/>
+      <c r="P14" s="46" t="n"/>
+      <c r="Q14" s="139" t="n"/>
+      <c r="R14" s="126" t="n"/>
+      <c r="S14" s="28" t="n"/>
+      <c r="T14" s="46" t="n"/>
+    </row>
+    <row r="15" ht="16" customHeight="1" s="121">
+      <c r="A15" s="140" t="n"/>
+      <c r="B15" s="126" t="n"/>
+      <c r="C15" s="28" t="n"/>
+      <c r="D15" s="46" t="n"/>
+      <c r="E15" s="139" t="n"/>
+      <c r="F15" s="126" t="n"/>
+      <c r="G15" s="28" t="n"/>
+      <c r="H15" s="46" t="n"/>
+      <c r="I15" s="139" t="n"/>
+      <c r="J15" s="126" t="n"/>
+      <c r="K15" s="28" t="n"/>
+      <c r="L15" s="46" t="n"/>
+      <c r="M15" s="138" t="n"/>
+      <c r="N15" s="126" t="n"/>
+      <c r="O15" s="28" t="n"/>
+      <c r="P15" s="46" t="n"/>
+      <c r="Q15" s="139" t="n"/>
+      <c r="R15" s="126" t="n"/>
+      <c r="S15" s="28" t="n"/>
+      <c r="T15" s="46" t="n"/>
+    </row>
+    <row r="16" ht="16" customHeight="1" s="121">
+      <c r="A16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="B16" s="126" t="n"/>
+      <c r="C16" s="147" t="n"/>
+      <c r="D16" s="52">
+        <f>SUM(D9:D14)</f>
+        <v/>
+      </c>
+      <c r="E16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="F16" s="126" t="n"/>
+      <c r="G16" s="147" t="n"/>
+      <c r="H16" s="52">
+        <f>SUM(H9:H12)</f>
+        <v/>
+      </c>
+      <c r="I16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="J16" s="126" t="n"/>
+      <c r="K16" s="147" t="n"/>
+      <c r="L16" s="52">
+        <f>SUM(L9:L12)</f>
+        <v/>
+      </c>
+      <c r="M16" s="143" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="N16" s="126" t="n"/>
+      <c r="O16" s="147" t="n"/>
+      <c r="P16" s="52">
+        <f>SUM(P9:P13)</f>
+        <v/>
+      </c>
+      <c r="Q16" s="156" t="inlineStr">
+        <is>
+          <t>Total Rounded</t>
+        </is>
+      </c>
+      <c r="R16" s="147" t="n"/>
+      <c r="S16" s="147" t="n"/>
+      <c r="T16" s="56">
+        <f>SUM(T9:T12)</f>
+        <v/>
+      </c>
+      <c r="U16" s="58" t="n"/>
+    </row>
+    <row r="17" ht="18" customHeight="1" s="121">
+      <c r="A17" s="214" t="n"/>
+      <c r="B17" s="128" t="n"/>
+      <c r="C17" s="128" t="n"/>
+      <c r="D17" s="128" t="n"/>
+      <c r="E17" s="128" t="n"/>
+      <c r="F17" s="128" t="n"/>
+      <c r="G17" s="128" t="n"/>
+      <c r="H17" s="128" t="n"/>
+      <c r="I17" s="128" t="n"/>
+      <c r="J17" s="128" t="n"/>
+      <c r="K17" s="128" t="n"/>
+      <c r="L17" s="128" t="n"/>
+      <c r="M17" s="128" t="n"/>
+      <c r="N17" s="128" t="n"/>
+      <c r="O17" s="128" t="n"/>
+      <c r="P17" s="128" t="n"/>
+      <c r="Q17" s="126" t="n"/>
+      <c r="R17" s="145" t="inlineStr">
+        <is>
+          <t>Earnings Saved:</t>
+        </is>
+      </c>
+      <c r="S17" s="126" t="n"/>
+      <c r="T17" s="215">
+        <f>SUM(D16,H16,L16,P16,T16)*20</f>
+        <v/>
+      </c>
+    </row>
+    <row r="18" ht="47" customHeight="1" s="121">
+      <c r="A18" s="141" t="inlineStr">
+        <is>
+          <t>Missing Clock Ins</t>
+        </is>
+      </c>
+      <c r="B18" s="126" t="n"/>
+      <c r="C18" s="134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Timesheets with recorded clock outs, but missing clock ins will be flagged and reported to managers. If no response is received, employees' scheduled clock in time will be manually entered. </t>
+        </is>
+      </c>
+      <c r="D18" s="128" t="n"/>
+      <c r="E18" s="128" t="n"/>
+      <c r="F18" s="128" t="n"/>
+      <c r="G18" s="128" t="n"/>
+      <c r="H18" s="128" t="n"/>
+      <c r="I18" s="128" t="n"/>
+      <c r="J18" s="128" t="n"/>
+      <c r="K18" s="128" t="n"/>
+      <c r="L18" s="128" t="n"/>
+      <c r="M18" s="128" t="n"/>
+      <c r="N18" s="128" t="n"/>
+      <c r="O18" s="128" t="n"/>
+      <c r="P18" s="128" t="n"/>
+      <c r="Q18" s="128" t="n"/>
+      <c r="R18" s="128" t="n"/>
+      <c r="S18" s="128" t="n"/>
+      <c r="T18" s="132" t="n"/>
+    </row>
+    <row r="19" ht="21" customHeight="1" s="121">
+      <c r="A19" s="91" t="n">
+        <v>12</v>
+      </c>
+      <c r="B19" s="30" t="n"/>
+      <c r="C19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="D19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="E19" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F19" s="30" t="n"/>
+      <c r="G19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="H19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="I19" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J19" s="30" t="n"/>
+      <c r="K19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="L19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="M19" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N19" s="30" t="n"/>
+      <c r="O19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="P19" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="Q19" s="92" t="n">
+        <v>16</v>
+      </c>
+      <c r="R19" s="92" t="n"/>
+      <c r="S19" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="T19" s="176" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+    </row>
+    <row r="20" ht="16" customHeight="1" s="121">
+      <c r="A20" s="137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">No Missing Clock Ins </t>
+        </is>
+      </c>
+      <c r="B20" s="126" t="n"/>
+      <c r="C20" s="147" t="n"/>
+      <c r="D20" s="27" t="n"/>
+      <c r="E20" s="142" t="n"/>
+      <c r="F20" s="126" t="n"/>
+      <c r="G20" s="147" t="n"/>
+      <c r="H20" s="27" t="n"/>
+      <c r="I20" s="142" t="n"/>
+      <c r="J20" s="126" t="n"/>
+      <c r="K20" s="147" t="n"/>
+      <c r="L20" s="171" t="n"/>
+      <c r="M20" s="142" t="n"/>
+      <c r="N20" s="126" t="n"/>
+      <c r="O20" s="28" t="n"/>
+      <c r="P20" s="171" t="n"/>
+      <c r="Q20" s="142" t="n"/>
+      <c r="R20" s="126" t="n"/>
+      <c r="S20" s="28" t="n"/>
+      <c r="T20" s="54" t="n"/>
+    </row>
+    <row r="21" ht="16" customHeight="1" s="121">
+      <c r="A21" s="146" t="n"/>
+      <c r="B21" s="126" t="n"/>
+      <c r="C21" s="28" t="n"/>
+      <c r="D21" s="171" t="n"/>
+      <c r="E21" s="142" t="n"/>
+      <c r="F21" s="126" t="n"/>
+      <c r="G21" s="28" t="n"/>
+      <c r="H21" s="171" t="n"/>
+      <c r="I21" s="147" t="n"/>
+      <c r="J21" s="126" t="n"/>
+      <c r="K21" s="147" t="n"/>
+      <c r="L21" s="147" t="n"/>
+      <c r="M21" s="147" t="n"/>
+      <c r="N21" s="126" t="n"/>
+      <c r="O21" s="147" t="n"/>
+      <c r="P21" s="147" t="n"/>
+      <c r="Q21" s="147" t="n"/>
+      <c r="R21" s="126" t="n"/>
+      <c r="S21" s="25" t="n"/>
+      <c r="T21" s="37" t="n"/>
+    </row>
+    <row r="22" ht="16" customHeight="1" s="121">
+      <c r="A22" s="140" t="n"/>
+      <c r="B22" s="126" t="n"/>
+      <c r="C22" s="147" t="n"/>
+      <c r="D22" s="147" t="n"/>
+      <c r="E22" s="142" t="n"/>
+      <c r="F22" s="126" t="n"/>
+      <c r="G22" s="28" t="n"/>
+      <c r="H22" s="28" t="n"/>
+      <c r="I22" s="147" t="n"/>
+      <c r="J22" s="126" t="n"/>
+      <c r="K22" s="147" t="n"/>
+      <c r="L22" s="147" t="n"/>
+      <c r="M22" s="147" t="n"/>
+      <c r="N22" s="126" t="n"/>
+      <c r="O22" s="147" t="n"/>
+      <c r="P22" s="147" t="n"/>
+      <c r="Q22" s="147" t="n"/>
+      <c r="R22" s="126" t="n"/>
+      <c r="S22" s="25" t="n"/>
+      <c r="T22" s="37" t="n"/>
+    </row>
+    <row r="23" ht="16" customHeight="1" s="121">
+      <c r="A23" s="140" t="n"/>
+      <c r="B23" s="126" t="n"/>
+      <c r="C23" s="147" t="n"/>
+      <c r="D23" s="147" t="n"/>
+      <c r="E23" s="142" t="n"/>
+      <c r="F23" s="126" t="n"/>
+      <c r="G23" s="28" t="n"/>
+      <c r="H23" s="28" t="n"/>
+      <c r="I23" s="147" t="n"/>
+      <c r="J23" s="126" t="n"/>
+      <c r="K23" s="147" t="n"/>
+      <c r="L23" s="147" t="n"/>
+      <c r="M23" s="147" t="n"/>
+      <c r="N23" s="126" t="n"/>
+      <c r="O23" s="147" t="n"/>
+      <c r="P23" s="147" t="n"/>
+      <c r="Q23" s="147" t="n"/>
+      <c r="R23" s="126" t="n"/>
+      <c r="S23" s="25" t="n"/>
+      <c r="T23" s="37" t="n"/>
+    </row>
+    <row r="24" ht="16" customHeight="1" s="121">
+      <c r="A24" s="140" t="n"/>
+      <c r="B24" s="126" t="n"/>
+      <c r="C24" s="147" t="n"/>
+      <c r="D24" s="147" t="n"/>
+      <c r="E24" s="142" t="n"/>
+      <c r="F24" s="126" t="n"/>
+      <c r="G24" s="28" t="n"/>
+      <c r="H24" s="147" t="n"/>
+      <c r="I24" s="147" t="n"/>
+      <c r="J24" s="126" t="n"/>
+      <c r="K24" s="147" t="n"/>
+      <c r="L24" s="147" t="n"/>
+      <c r="M24" s="147" t="n"/>
+      <c r="N24" s="126" t="n"/>
+      <c r="O24" s="147" t="n"/>
+      <c r="P24" s="147" t="n"/>
+      <c r="Q24" s="147" t="n"/>
+      <c r="R24" s="126" t="n"/>
+      <c r="S24" s="25" t="n"/>
+      <c r="T24" s="37" t="n"/>
+    </row>
+    <row r="25" ht="17" customHeight="1" s="121">
+      <c r="A25" s="148" t="n"/>
+      <c r="B25" s="128" t="n"/>
+      <c r="C25" s="128" t="n"/>
+      <c r="D25" s="128" t="n"/>
+      <c r="E25" s="128" t="n"/>
+      <c r="F25" s="128" t="n"/>
+      <c r="G25" s="128" t="n"/>
+      <c r="H25" s="128" t="n"/>
+      <c r="I25" s="128" t="n"/>
+      <c r="J25" s="128" t="n"/>
+      <c r="K25" s="128" t="n"/>
+      <c r="L25" s="128" t="n"/>
+      <c r="M25" s="128" t="n"/>
+      <c r="N25" s="128" t="n"/>
+      <c r="O25" s="128" t="n"/>
+      <c r="P25" s="128" t="n"/>
+      <c r="Q25" s="128" t="n"/>
+      <c r="R25" s="128" t="n"/>
+      <c r="S25" s="128" t="n"/>
+      <c r="T25" s="132" t="n"/>
+    </row>
+    <row r="26" ht="44" customHeight="1" s="121">
+      <c r="A26" s="141" t="inlineStr">
+        <is>
+          <t>Missing Clock Outs</t>
+        </is>
+      </c>
+      <c r="B26" s="126" t="n"/>
+      <c r="C26" s="134" t="inlineStr">
+        <is>
+          <t>Timesheets with recorded Clock Ins but missing clock outs will be flagged and reported to managers. If no response is received, employees' scheduled clock-out  will be manually eneterd.</t>
+        </is>
+      </c>
+      <c r="D26" s="128" t="n"/>
+      <c r="E26" s="128" t="n"/>
+      <c r="F26" s="128" t="n"/>
+      <c r="G26" s="128" t="n"/>
+      <c r="H26" s="128" t="n"/>
+      <c r="I26" s="128" t="n"/>
+      <c r="J26" s="128" t="n"/>
+      <c r="K26" s="128" t="n"/>
+      <c r="L26" s="128" t="n"/>
+      <c r="M26" s="128" t="n"/>
+      <c r="N26" s="128" t="n"/>
+      <c r="O26" s="128" t="n"/>
+      <c r="P26" s="128" t="n"/>
+      <c r="Q26" s="128" t="n"/>
+      <c r="R26" s="128" t="n"/>
+      <c r="S26" s="128" t="n"/>
+      <c r="T26" s="132" t="n"/>
+    </row>
+    <row r="27" ht="21" customHeight="1" s="121">
+      <c r="A27" s="91" t="n">
+        <v>12</v>
+      </c>
+      <c r="B27" s="30" t="n"/>
+      <c r="C27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="D27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="E27" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F27" s="30" t="n"/>
+      <c r="G27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="H27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="I27" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J27" s="30" t="n"/>
+      <c r="K27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="L27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="M27" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N27" s="30" t="n"/>
+      <c r="O27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="P27" s="180" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+      <c r="Q27" s="93" t="n">
+        <v>16</v>
+      </c>
+      <c r="R27" s="94" t="n"/>
+      <c r="S27" s="180" t="inlineStr">
+        <is>
+          <t xml:space="preserve">in </t>
+        </is>
+      </c>
+      <c r="T27" s="176" t="inlineStr">
+        <is>
+          <t>out</t>
+        </is>
+      </c>
+    </row>
+    <row r="28" ht="16" customHeight="1" s="121">
+      <c r="A28" s="149" t="inlineStr">
+        <is>
+          <t>No Missing Clock Outs</t>
+        </is>
+      </c>
+      <c r="B28" s="126" t="n"/>
+      <c r="C28" s="28" t="n"/>
+      <c r="D28" s="51" t="n"/>
+      <c r="E28" s="150" t="n"/>
+      <c r="F28" s="126" t="n"/>
+      <c r="G28" s="28" t="n"/>
+      <c r="H28" s="28" t="n"/>
+      <c r="I28" s="150" t="n"/>
+      <c r="J28" s="126" t="n"/>
+      <c r="K28" s="28" t="n"/>
+      <c r="L28" s="147" t="n"/>
+      <c r="M28" s="150" t="n"/>
+      <c r="N28" s="126" t="n"/>
+      <c r="O28" s="28" t="n"/>
+      <c r="P28" s="28" t="n"/>
+      <c r="Q28" s="149" t="n"/>
+      <c r="R28" s="126" t="n"/>
+      <c r="S28" s="28" t="n"/>
+      <c r="T28" s="54" t="n"/>
+    </row>
+    <row r="29" ht="16" customHeight="1" s="121">
+      <c r="A29" s="150" t="n"/>
+      <c r="B29" s="126" t="n"/>
+      <c r="C29" s="28" t="n"/>
+      <c r="D29" s="147" t="n"/>
+      <c r="E29" s="150" t="n"/>
+      <c r="F29" s="126" t="n"/>
+      <c r="G29" s="28" t="n"/>
+      <c r="H29" s="28" t="n"/>
+      <c r="I29" s="147" t="n"/>
+      <c r="J29" s="126" t="n"/>
+      <c r="K29" s="147" t="n"/>
+      <c r="L29" s="147" t="n"/>
+      <c r="M29" s="151" t="n"/>
+      <c r="N29" s="126" t="n"/>
+      <c r="O29" s="147" t="n"/>
+      <c r="P29" s="147" t="n"/>
+      <c r="Q29" s="147" t="n"/>
+      <c r="R29" s="126" t="n"/>
+      <c r="S29" s="28" t="n"/>
+      <c r="T29" s="35" t="n"/>
+    </row>
+    <row r="30" ht="16" customHeight="1" s="121">
+      <c r="A30" s="140" t="n"/>
+      <c r="B30" s="126" t="n"/>
+      <c r="C30" s="147" t="n"/>
+      <c r="D30" s="147" t="n"/>
+      <c r="E30" s="142" t="n"/>
+      <c r="F30" s="126" t="n"/>
+      <c r="G30" s="28" t="n"/>
+      <c r="H30" s="28" t="n"/>
+      <c r="I30" s="147" t="n"/>
+      <c r="J30" s="126" t="n"/>
+      <c r="K30" s="147" t="n"/>
+      <c r="L30" s="147" t="n"/>
+      <c r="M30" s="152" t="n"/>
+      <c r="N30" s="126" t="n"/>
+      <c r="O30" s="28" t="n"/>
+      <c r="P30" s="147" t="n"/>
+      <c r="Q30" s="147" t="n"/>
+      <c r="R30" s="126" t="n"/>
+      <c r="S30" s="147" t="n"/>
+      <c r="T30" s="35" t="n"/>
+    </row>
+    <row r="31" ht="16" customHeight="1" s="121">
+      <c r="A31" s="140" t="n"/>
+      <c r="B31" s="126" t="n"/>
+      <c r="C31" s="147" t="n"/>
+      <c r="D31" s="147" t="n"/>
+      <c r="E31" s="142" t="n"/>
+      <c r="F31" s="126" t="n"/>
+      <c r="G31" s="28" t="n"/>
+      <c r="H31" s="28" t="n"/>
+      <c r="I31" s="147" t="n"/>
+      <c r="J31" s="126" t="n"/>
+      <c r="K31" s="147" t="n"/>
+      <c r="L31" s="147" t="n"/>
+      <c r="M31" s="152" t="n"/>
+      <c r="N31" s="126" t="n"/>
+      <c r="O31" s="28" t="n"/>
+      <c r="P31" s="147" t="n"/>
+      <c r="Q31" s="147" t="n"/>
+      <c r="R31" s="126" t="n"/>
+      <c r="S31" s="147" t="n"/>
+      <c r="T31" s="35" t="n"/>
+    </row>
+    <row r="32" ht="16" customHeight="1" s="121">
+      <c r="A32" s="140" t="n"/>
+      <c r="B32" s="126" t="n"/>
+      <c r="C32" s="147" t="n"/>
+      <c r="D32" s="147" t="n"/>
+      <c r="E32" s="142" t="n"/>
+      <c r="F32" s="126" t="n"/>
+      <c r="G32" s="28" t="n"/>
+      <c r="H32" s="147" t="n"/>
+      <c r="I32" s="147" t="n"/>
+      <c r="J32" s="126" t="n"/>
+      <c r="K32" s="147" t="n"/>
+      <c r="L32" s="147" t="n"/>
+      <c r="M32" s="152" t="n"/>
+      <c r="N32" s="126" t="n"/>
+      <c r="O32" s="28" t="n"/>
+      <c r="P32" s="147" t="n"/>
+      <c r="Q32" s="147" t="n"/>
+      <c r="R32" s="126" t="n"/>
+      <c r="S32" s="147" t="n"/>
+      <c r="T32" s="35" t="n"/>
+    </row>
+    <row r="33" ht="19" customHeight="1" s="121">
+      <c r="A33" s="148" t="n"/>
+      <c r="B33" s="128" t="n"/>
+      <c r="C33" s="128" t="n"/>
+      <c r="D33" s="128" t="n"/>
+      <c r="E33" s="128" t="n"/>
+      <c r="F33" s="128" t="n"/>
+      <c r="G33" s="128" t="n"/>
+      <c r="H33" s="128" t="n"/>
+      <c r="I33" s="128" t="n"/>
+      <c r="J33" s="128" t="n"/>
+      <c r="K33" s="128" t="n"/>
+      <c r="L33" s="128" t="n"/>
+      <c r="M33" s="128" t="n"/>
+      <c r="N33" s="128" t="n"/>
+      <c r="O33" s="128" t="n"/>
+      <c r="P33" s="128" t="n"/>
+      <c r="Q33" s="128" t="n"/>
+      <c r="R33" s="128" t="n"/>
+      <c r="S33" s="128" t="n"/>
+      <c r="T33" s="132" t="n"/>
+    </row>
+    <row r="34" ht="23.25" customHeight="1" s="121">
+      <c r="A34" s="133" t="inlineStr">
+        <is>
+          <t>Absences</t>
+        </is>
+      </c>
+      <c r="B34" s="126" t="n"/>
+      <c r="C34" s="153" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Absences will be reported to managers when an employee with a fixed schedule fails to clock in or out during their scheudled shift.  </t>
+        </is>
+      </c>
+      <c r="D34" s="128" t="n"/>
+      <c r="E34" s="128" t="n"/>
+      <c r="F34" s="128" t="n"/>
+      <c r="G34" s="128" t="n"/>
+      <c r="H34" s="128" t="n"/>
+      <c r="I34" s="128" t="n"/>
+      <c r="J34" s="128" t="n"/>
+      <c r="K34" s="128" t="n"/>
+      <c r="L34" s="128" t="n"/>
+      <c r="M34" s="128" t="n"/>
+      <c r="N34" s="128" t="n"/>
+      <c r="O34" s="128" t="n"/>
+      <c r="P34" s="128" t="n"/>
+      <c r="Q34" s="128" t="n"/>
+      <c r="R34" s="128" t="n"/>
+      <c r="S34" s="128" t="n"/>
+      <c r="T34" s="132" t="n"/>
+    </row>
+    <row r="35" ht="18.75" customHeight="1" s="121">
+      <c r="A35" s="91" t="n">
+        <v>12</v>
+      </c>
+      <c r="B35" s="30" t="n"/>
+      <c r="C35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="D35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="E35" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F35" s="30" t="n"/>
+      <c r="G35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="H35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="I35" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J35" s="30" t="n"/>
+      <c r="K35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="L35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="M35" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N35" s="30" t="n"/>
+      <c r="O35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="P35" s="180" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="Q35" s="93" t="n">
+        <v>16</v>
+      </c>
+      <c r="R35" s="94" t="n"/>
+      <c r="S35" s="180" t="inlineStr">
+        <is>
+          <t>In</t>
+        </is>
+      </c>
+      <c r="T35" s="176" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+    </row>
+    <row r="36" ht="15.75" customHeight="1" s="121">
+      <c r="A36" s="137" t="inlineStr">
+        <is>
+          <t>No Absences</t>
+        </is>
+      </c>
+      <c r="B36" s="126" t="n"/>
+      <c r="C36" s="95" t="n"/>
+      <c r="D36" s="95" t="n"/>
+      <c r="E36" s="142" t="n"/>
+      <c r="F36" s="126" t="n"/>
+      <c r="G36" s="95" t="n"/>
+      <c r="H36" s="95" t="n"/>
+      <c r="I36" s="142" t="n"/>
+      <c r="J36" s="126" t="n"/>
+      <c r="K36" s="95" t="n"/>
+      <c r="L36" s="95" t="n"/>
+      <c r="M36" s="142" t="n"/>
+      <c r="N36" s="126" t="n"/>
+      <c r="O36" s="95" t="n"/>
+      <c r="P36" s="95" t="n"/>
+      <c r="Q36" s="142" t="n"/>
+      <c r="R36" s="126" t="n"/>
+      <c r="S36" s="95" t="n"/>
+      <c r="T36" s="96" t="n"/>
+    </row>
+    <row r="37" ht="15.75" customHeight="1" s="121">
+      <c r="A37" s="140" t="n"/>
+      <c r="B37" s="126" t="n"/>
+      <c r="C37" s="95" t="n"/>
+      <c r="D37" s="95" t="n"/>
+      <c r="E37" s="142" t="n"/>
+      <c r="F37" s="126" t="n"/>
+      <c r="G37" s="95" t="n"/>
+      <c r="H37" s="95" t="n"/>
+      <c r="I37" s="147" t="n"/>
+      <c r="J37" s="126" t="n"/>
+      <c r="K37" s="95" t="n"/>
+      <c r="L37" s="95" t="n"/>
+      <c r="M37" s="152" t="n"/>
+      <c r="N37" s="126" t="n"/>
+      <c r="O37" s="95" t="n"/>
+      <c r="P37" s="95" t="n"/>
+      <c r="Q37" s="152" t="n"/>
+      <c r="R37" s="126" t="n"/>
+      <c r="S37" s="95" t="n"/>
+      <c r="T37" s="96" t="n"/>
+    </row>
+    <row r="38" ht="15.75" customHeight="1" s="121">
+      <c r="A38" s="140" t="n"/>
+      <c r="B38" s="126" t="n"/>
+      <c r="C38" s="95" t="n"/>
+      <c r="D38" s="95" t="n"/>
+      <c r="E38" s="142" t="n"/>
+      <c r="F38" s="126" t="n"/>
+      <c r="G38" s="95" t="n"/>
+      <c r="H38" s="95" t="n"/>
+      <c r="I38" s="147" t="n"/>
+      <c r="J38" s="126" t="n"/>
+      <c r="K38" s="95" t="n"/>
+      <c r="L38" s="95" t="n"/>
+      <c r="M38" s="152" t="n"/>
+      <c r="N38" s="126" t="n"/>
+      <c r="O38" s="95" t="n"/>
+      <c r="P38" s="95" t="n"/>
+      <c r="Q38" s="152" t="n"/>
+      <c r="R38" s="126" t="n"/>
+      <c r="S38" s="95" t="n"/>
+      <c r="T38" s="96" t="n"/>
+    </row>
+    <row r="39" ht="15.75" customHeight="1" s="121">
+      <c r="A39" s="140" t="n"/>
+      <c r="B39" s="126" t="n"/>
+      <c r="C39" s="95" t="n"/>
+      <c r="D39" s="95" t="n"/>
+      <c r="E39" s="142" t="n"/>
+      <c r="F39" s="126" t="n"/>
+      <c r="G39" s="95" t="n"/>
+      <c r="H39" s="95" t="n"/>
+      <c r="I39" s="147" t="n"/>
+      <c r="J39" s="126" t="n"/>
+      <c r="K39" s="95" t="n"/>
+      <c r="L39" s="95" t="n"/>
+      <c r="M39" s="152" t="n"/>
+      <c r="N39" s="126" t="n"/>
+      <c r="O39" s="95" t="n"/>
+      <c r="P39" s="95" t="n"/>
+      <c r="Q39" s="152" t="n"/>
+      <c r="R39" s="126" t="n"/>
+      <c r="S39" s="95" t="n"/>
+      <c r="T39" s="96" t="n"/>
+    </row>
+    <row r="40" ht="15.75" customHeight="1" s="121">
+      <c r="A40" s="140" t="n"/>
+      <c r="B40" s="126" t="n"/>
+      <c r="C40" s="95" t="n"/>
+      <c r="D40" s="95" t="n"/>
+      <c r="E40" s="142" t="n"/>
+      <c r="F40" s="126" t="n"/>
+      <c r="G40" s="95" t="n"/>
+      <c r="H40" s="95" t="n"/>
+      <c r="I40" s="147" t="n"/>
+      <c r="J40" s="126" t="n"/>
+      <c r="K40" s="95" t="n"/>
+      <c r="L40" s="95" t="n"/>
+      <c r="M40" s="152" t="n"/>
+      <c r="N40" s="126" t="n"/>
+      <c r="O40" s="95" t="n"/>
+      <c r="P40" s="95" t="n"/>
+      <c r="Q40" s="152" t="n"/>
+      <c r="R40" s="126" t="n"/>
+      <c r="S40" s="95" t="n"/>
+      <c r="T40" s="96" t="n"/>
+    </row>
+    <row r="41" ht="17" customHeight="1" s="121">
+      <c r="A41" s="148" t="n"/>
+      <c r="B41" s="128" t="n"/>
+      <c r="C41" s="128" t="n"/>
+      <c r="D41" s="128" t="n"/>
+      <c r="E41" s="128" t="n"/>
+      <c r="F41" s="128" t="n"/>
+      <c r="G41" s="128" t="n"/>
+      <c r="H41" s="128" t="n"/>
+      <c r="I41" s="128" t="n"/>
+      <c r="J41" s="128" t="n"/>
+      <c r="K41" s="128" t="n"/>
+      <c r="L41" s="128" t="n"/>
+      <c r="M41" s="128" t="n"/>
+      <c r="N41" s="128" t="n"/>
+      <c r="O41" s="128" t="n"/>
+      <c r="P41" s="128" t="n"/>
+      <c r="Q41" s="128" t="n"/>
+      <c r="R41" s="128" t="n"/>
+      <c r="S41" s="128" t="n"/>
+      <c r="T41" s="132" t="n"/>
+    </row>
+    <row r="42" ht="43.5" customHeight="1" s="121">
+      <c r="A42" s="154" t="inlineStr">
+        <is>
+          <t>Additional Hours Worked</t>
+        </is>
+      </c>
+      <c r="B42" s="126" t="n"/>
+      <c r="C42" s="134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Timesheets with clock-outs that exceed 2+ hours of scheduled clock-out time will flagged by HomeBase and reported to managers. If no response is received, administrative action will not be taken and clock out time will be left as is. </t>
+        </is>
+      </c>
+      <c r="D42" s="128" t="n"/>
+      <c r="E42" s="128" t="n"/>
+      <c r="F42" s="128" t="n"/>
+      <c r="G42" s="128" t="n"/>
+      <c r="H42" s="128" t="n"/>
+      <c r="I42" s="128" t="n"/>
+      <c r="J42" s="128" t="n"/>
+      <c r="K42" s="128" t="n"/>
+      <c r="L42" s="128" t="n"/>
+      <c r="M42" s="128" t="n"/>
+      <c r="N42" s="128" t="n"/>
+      <c r="O42" s="128" t="n"/>
+      <c r="P42" s="128" t="n"/>
+      <c r="Q42" s="128" t="n"/>
+      <c r="R42" s="128" t="n"/>
+      <c r="S42" s="128" t="n"/>
+      <c r="T42" s="132" t="n"/>
+    </row>
+    <row r="43" ht="21" customHeight="1" s="121">
+      <c r="A43" s="97" t="n">
+        <v>12</v>
+      </c>
+      <c r="B43" s="98" t="n"/>
+      <c r="C43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="D43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="E43" s="88" t="n">
+        <v>13</v>
+      </c>
+      <c r="F43" s="30" t="n"/>
+      <c r="G43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="H43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="I43" s="88" t="n">
+        <v>14</v>
+      </c>
+      <c r="J43" s="30" t="n"/>
+      <c r="K43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="L43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="M43" s="88" t="n">
+        <v>15</v>
+      </c>
+      <c r="N43" s="30" t="n"/>
+      <c r="O43" s="99" t="inlineStr">
+        <is>
+          <t>Out</t>
+        </is>
+      </c>
+      <c r="P43" s="99" t="inlineStr">
+        <is>
+          <t>Hrs</t>
+        </is>
+      </c>
+      <c r="Q43" s="93" t="n">
+        <v>16</v>
       </c>
       <c r="R43" s="94" t="n"/>
       <c r="S43" s="99" t="inlineStr">

</xml_diff>

<commit_message>
Created get_missing_punches() in populate.py
</commit_message>
<xml_diff>
--- a/TimeReportLog(Oct2022).xlsx
+++ b/TimeReportLog(Oct2022).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lije/Desktop/Software-Development/Chaz-Project/auto-ace/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Noah\coding-projects\ace-time-reporting\xl-data-auto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD2062E-5B4E-4745-86A3-3B243432DF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FBB020-A3C7-4CF5-8D6F-C427DE73CC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Weekly Time Reporting Template" sheetId="1" r:id="rId1"/>
@@ -2887,28 +2887,28 @@
       <selection activeCell="M16" sqref="M16:N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="4" width="8.31640625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" customWidth="1"/>
+    <col min="8" max="8" width="8.1796875" customWidth="1"/>
     <col min="9" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="7.5" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7.6796875" customWidth="1"/>
+    <col min="15" max="15" width="7.31640625" customWidth="1"/>
     <col min="16" max="16" width="7.5" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.1796875" customWidth="1"/>
+    <col min="19" max="19" width="5.6796875" customWidth="1"/>
+    <col min="20" max="20" width="8.31640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="157" t="s">
         <v>0</v>
       </c>
@@ -2934,7 +2934,7 @@
       <c r="S1" s="160"/>
       <c r="T1" s="161"/>
     </row>
-    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="166"/>
       <c r="B2" s="121"/>
       <c r="C2" s="96" t="s">
@@ -2964,7 +2964,7 @@
       <c r="S2" s="162"/>
       <c r="T2" s="163"/>
     </row>
-    <row r="3" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="168" t="s">
         <v>5</v>
       </c>
@@ -2995,7 +2995,7 @@
       <c r="S3" s="162"/>
       <c r="T3" s="163"/>
     </row>
-    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="168" t="s">
         <v>7</v>
       </c>
@@ -3026,7 +3026,7 @@
       <c r="S4" s="162"/>
       <c r="T4" s="163"/>
     </row>
-    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="168" t="s">
         <v>9</v>
       </c>
@@ -3057,7 +3057,7 @@
       <c r="S5" s="164"/>
       <c r="T5" s="165"/>
     </row>
-    <row r="6" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="1">
       <c r="A6" s="154"/>
       <c r="B6" s="135"/>
       <c r="C6" s="135"/>
@@ -3079,7 +3079,7 @@
       <c r="S6" s="135"/>
       <c r="T6" s="136"/>
     </row>
-    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="143" t="s">
         <v>11</v>
       </c>
@@ -3105,7 +3105,7 @@
       <c r="S7" s="135"/>
       <c r="T7" s="136"/>
     </row>
-    <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="155">
         <v>17</v>
       </c>
@@ -3161,7 +3161,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="145" t="s">
         <v>15</v>
       </c>
@@ -3190,7 +3190,7 @@
       <c r="S9" s="116"/>
       <c r="T9" s="36"/>
     </row>
-    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="153"/>
       <c r="B10" s="121"/>
       <c r="C10" s="116"/>
@@ -3215,7 +3215,7 @@
       <c r="S10" s="116"/>
       <c r="T10" s="70"/>
     </row>
-    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="153"/>
       <c r="B11" s="121"/>
       <c r="C11" s="116"/>
@@ -3240,7 +3240,7 @@
       <c r="S11" s="116"/>
       <c r="T11" s="71"/>
     </row>
-    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="152"/>
       <c r="B12" s="121"/>
       <c r="C12" s="116"/>
@@ -3265,7 +3265,7 @@
       <c r="S12" s="116"/>
       <c r="T12" s="70"/>
     </row>
-    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="153"/>
       <c r="B13" s="121"/>
       <c r="C13" s="116"/>
@@ -3290,7 +3290,7 @@
       <c r="S13" s="116"/>
       <c r="T13" s="70"/>
     </row>
-    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="152"/>
       <c r="B14" s="121"/>
       <c r="C14" s="116"/>
@@ -3315,7 +3315,7 @@
       <c r="S14" s="116"/>
       <c r="T14" s="70"/>
     </row>
-    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="139"/>
       <c r="B15" s="121"/>
       <c r="C15" s="116"/>
@@ -3340,7 +3340,7 @@
       <c r="S15" s="116"/>
       <c r="T15" s="70"/>
     </row>
-    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="124" t="s">
         <v>16</v>
       </c>
@@ -3388,7 +3388,7 @@
       </c>
       <c r="U16" s="92"/>
     </row>
-    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="150"/>
       <c r="B17" s="135"/>
       <c r="C17" s="135"/>
@@ -3415,7 +3415,7 @@
         <v>3.3333333333333215</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="47" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="47" customHeight="1" x14ac:dyDescent="1">
       <c r="A18" s="147" t="s">
         <v>18</v>
       </c>
@@ -3441,7 +3441,7 @@
       <c r="S18" s="135"/>
       <c r="T18" s="136"/>
     </row>
-    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="52">
         <v>17</v>
       </c>
@@ -3497,7 +3497,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="145" t="s">
         <v>22</v>
       </c>
@@ -3521,7 +3521,7 @@
       <c r="S20" s="38"/>
       <c r="T20" s="85"/>
     </row>
-    <row r="21" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="149"/>
       <c r="B21" s="121"/>
       <c r="C21" s="38"/>
@@ -3543,7 +3543,7 @@
       <c r="S21" s="33"/>
       <c r="T21" s="57"/>
     </row>
-    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="139"/>
       <c r="B22" s="121"/>
       <c r="C22" s="36"/>
@@ -3565,7 +3565,7 @@
       <c r="S22" s="33"/>
       <c r="T22" s="57"/>
     </row>
-    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="139"/>
       <c r="B23" s="121"/>
       <c r="C23" s="36"/>
@@ -3587,7 +3587,7 @@
       <c r="S23" s="33"/>
       <c r="T23" s="57"/>
     </row>
-    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="139"/>
       <c r="B24" s="121"/>
       <c r="C24" s="36"/>
@@ -3609,7 +3609,7 @@
       <c r="S24" s="33"/>
       <c r="T24" s="57"/>
     </row>
-    <row r="25" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="134"/>
       <c r="B25" s="135"/>
       <c r="C25" s="135"/>
@@ -3631,7 +3631,7 @@
       <c r="S25" s="135"/>
       <c r="T25" s="136"/>
     </row>
-    <row r="26" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="1">
       <c r="A26" s="147" t="s">
         <v>23</v>
       </c>
@@ -3657,7 +3657,7 @@
       <c r="S26" s="135"/>
       <c r="T26" s="136"/>
     </row>
-    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="52">
         <v>17</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="148" t="s">
         <v>25</v>
       </c>
@@ -3737,7 +3737,7 @@
       <c r="S28" s="38"/>
       <c r="T28" s="85"/>
     </row>
-    <row r="29" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="146"/>
       <c r="B29" s="121"/>
       <c r="C29" s="38"/>
@@ -3759,7 +3759,7 @@
       <c r="S29" s="38"/>
       <c r="T29" s="55"/>
     </row>
-    <row r="30" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="139"/>
       <c r="B30" s="121"/>
       <c r="C30" s="36"/>
@@ -3781,7 +3781,7 @@
       <c r="S30" s="36"/>
       <c r="T30" s="55"/>
     </row>
-    <row r="31" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="139"/>
       <c r="B31" s="121"/>
       <c r="C31" s="36"/>
@@ -3803,7 +3803,7 @@
       <c r="S31" s="36"/>
       <c r="T31" s="55"/>
     </row>
-    <row r="32" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="139"/>
       <c r="B32" s="121"/>
       <c r="C32" s="36"/>
@@ -3825,7 +3825,7 @@
       <c r="S32" s="36"/>
       <c r="T32" s="55"/>
     </row>
-    <row r="33" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="134"/>
       <c r="B33" s="135"/>
       <c r="C33" s="135"/>
@@ -3847,7 +3847,7 @@
       <c r="S33" s="135"/>
       <c r="T33" s="136"/>
     </row>
-    <row r="34" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A34" s="143" t="s">
         <v>26</v>
       </c>
@@ -3873,7 +3873,7 @@
       <c r="S34" s="135"/>
       <c r="T34" s="136"/>
     </row>
-    <row r="35" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A35" s="52">
         <v>17</v>
       </c>
@@ -3929,7 +3929,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="145" t="s">
         <v>30</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="S36" s="69"/>
       <c r="T36" s="83"/>
     </row>
-    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="139"/>
       <c r="B37" s="121"/>
       <c r="C37" s="69"/>
@@ -3975,7 +3975,7 @@
       <c r="S37" s="69"/>
       <c r="T37" s="83"/>
     </row>
-    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A38" s="139"/>
       <c r="B38" s="121"/>
       <c r="C38" s="69"/>
@@ -3997,7 +3997,7 @@
       <c r="S38" s="69"/>
       <c r="T38" s="83"/>
     </row>
-    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="139"/>
       <c r="B39" s="121"/>
       <c r="C39" s="69"/>
@@ -4019,7 +4019,7 @@
       <c r="S39" s="69"/>
       <c r="T39" s="83"/>
     </row>
-    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="139"/>
       <c r="B40" s="121"/>
       <c r="C40" s="69"/>
@@ -4041,7 +4041,7 @@
       <c r="S40" s="69"/>
       <c r="T40" s="83"/>
     </row>
-    <row r="41" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A41" s="134"/>
       <c r="B41" s="135"/>
       <c r="C41" s="135"/>
@@ -4063,7 +4063,7 @@
       <c r="S41" s="135"/>
       <c r="T41" s="136"/>
     </row>
-    <row r="42" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="137" t="s">
         <v>31</v>
       </c>
@@ -4089,7 +4089,7 @@
       <c r="S42" s="135"/>
       <c r="T42" s="136"/>
     </row>
-    <row r="43" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="87">
         <v>17</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="132" t="s">
         <v>34</v>
       </c>
@@ -4169,7 +4169,7 @@
       <c r="S44" s="38"/>
       <c r="T44" s="85"/>
     </row>
-    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A45" s="123"/>
       <c r="B45" s="121"/>
       <c r="C45" s="51"/>
@@ -4191,7 +4191,7 @@
       <c r="S45" s="69"/>
       <c r="T45" s="83"/>
     </row>
-    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A46" s="123"/>
       <c r="B46" s="121"/>
       <c r="C46" s="51"/>
@@ -4212,7 +4212,7 @@
       <c r="S46" s="69"/>
       <c r="T46" s="83"/>
     </row>
-    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="123"/>
       <c r="B47" s="121"/>
       <c r="C47" s="51"/>
@@ -4234,7 +4234,7 @@
       <c r="S47" s="69"/>
       <c r="T47" s="83"/>
     </row>
-    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A48" s="124"/>
       <c r="B48" s="121"/>
       <c r="C48" s="73"/>
@@ -4256,7 +4256,7 @@
       <c r="S48" s="69"/>
       <c r="T48" s="83"/>
     </row>
-    <row r="49" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="123"/>
       <c r="B49" s="121"/>
       <c r="C49" s="73"/>
@@ -4278,7 +4278,7 @@
       <c r="S49" s="46"/>
       <c r="T49" s="68"/>
     </row>
-    <row r="50" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="123"/>
       <c r="B50" s="121"/>
       <c r="C50" s="73"/>
@@ -4300,7 +4300,7 @@
       <c r="S50" s="46"/>
       <c r="T50" s="68"/>
     </row>
-    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A51" s="123"/>
       <c r="B51" s="121"/>
       <c r="C51" s="73"/>
@@ -4322,7 +4322,7 @@
       <c r="S51" s="46"/>
       <c r="T51" s="68"/>
     </row>
-    <row r="52" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A52" s="122" t="s">
         <v>16</v>
       </c>
@@ -4369,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A53" s="128"/>
       <c r="B53" s="129"/>
       <c r="C53" s="129"/>
@@ -4700,22 +4700,22 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="5.31640625" customWidth="1"/>
     <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="6" max="6" width="9.83203125" customWidth="1"/>
+    <col min="6" max="6" width="9.81640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="5.6640625" customWidth="1"/>
+    <col min="8" max="8" width="5.6796875" customWidth="1"/>
     <col min="11" max="11" width="5.5" customWidth="1"/>
-    <col min="12" max="12" width="6.33203125" customWidth="1"/>
+    <col min="12" max="12" width="6.31640625" customWidth="1"/>
     <col min="15" max="16" width="5.5" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" customWidth="1"/>
+    <col min="19" max="19" width="5.6796875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="50.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="178" t="s">
         <v>36</v>
       </c>
@@ -4739,7 +4739,7 @@
       <c r="S1" s="158"/>
       <c r="T1" s="179"/>
     </row>
-    <row r="2" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="1">
       <c r="A2" s="154"/>
       <c r="B2" s="135"/>
       <c r="C2" s="135"/>
@@ -4761,7 +4761,7 @@
       <c r="S2" s="135"/>
       <c r="T2" s="136"/>
     </row>
-    <row r="3" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="1">
       <c r="A3" s="147" t="s">
         <v>11</v>
       </c>
@@ -4790,7 +4790,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="52">
         <v>10</v>
       </c>
@@ -4849,7 +4849,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="124" t="s">
         <v>38</v>
       </c>
@@ -4889,7 +4889,7 @@
       <c r="S5" s="36"/>
       <c r="T5" s="55"/>
     </row>
-    <row r="6" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A6" s="124" t="s">
         <v>41</v>
       </c>
@@ -4923,7 +4923,7 @@
       <c r="S6" s="36"/>
       <c r="T6" s="55"/>
     </row>
-    <row r="7" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="124" t="s">
         <v>42</v>
       </c>
@@ -4957,7 +4957,7 @@
       <c r="S7" s="36"/>
       <c r="T7" s="55"/>
     </row>
-    <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A8" s="139"/>
       <c r="B8" s="121"/>
       <c r="C8" s="115"/>
@@ -4985,7 +4985,7 @@
       <c r="S8" s="36"/>
       <c r="T8" s="55"/>
     </row>
-    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A9" s="139"/>
       <c r="B9" s="121"/>
       <c r="C9" s="115"/>
@@ -5013,7 +5013,7 @@
       <c r="S9" s="36"/>
       <c r="T9" s="55"/>
     </row>
-    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A10" s="124" t="s">
         <v>16</v>
       </c>
@@ -5060,7 +5060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" ht="33" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="90"/>
       <c r="B11" s="49"/>
       <c r="C11" s="49"/>
@@ -5087,7 +5087,7 @@
         <v>177.93199999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" ht="47" customHeight="1" x14ac:dyDescent="1">
       <c r="A12" s="147" t="s">
         <v>18</v>
       </c>
@@ -5113,7 +5113,7 @@
       <c r="S12" s="135"/>
       <c r="T12" s="136"/>
     </row>
-    <row r="13" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="52">
         <v>10</v>
       </c>
@@ -5169,7 +5169,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="124" t="s">
         <v>22</v>
       </c>
@@ -5201,7 +5201,7 @@
       <c r="S14" s="46"/>
       <c r="T14" s="56"/>
     </row>
-    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="149"/>
       <c r="B15" s="121"/>
       <c r="C15" s="38"/>
@@ -5223,7 +5223,7 @@
       <c r="S15" s="33"/>
       <c r="T15" s="57"/>
     </row>
-    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="139"/>
       <c r="B16" s="121"/>
       <c r="C16" s="36"/>
@@ -5245,7 +5245,7 @@
       <c r="S16" s="33"/>
       <c r="T16" s="57"/>
     </row>
-    <row r="17" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="139"/>
       <c r="B17" s="121"/>
       <c r="C17" s="36"/>
@@ -5267,7 +5267,7 @@
       <c r="S17" s="33"/>
       <c r="T17" s="57"/>
     </row>
-    <row r="18" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A18" s="139"/>
       <c r="B18" s="121"/>
       <c r="C18" s="36"/>
@@ -5289,7 +5289,7 @@
       <c r="S18" s="33"/>
       <c r="T18" s="57"/>
     </row>
-    <row r="19" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="31" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="134"/>
       <c r="B19" s="135"/>
       <c r="C19" s="135"/>
@@ -5311,7 +5311,7 @@
       <c r="S19" s="135"/>
       <c r="T19" s="136"/>
     </row>
-    <row r="20" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="1">
       <c r="A20" s="147" t="s">
         <v>23</v>
       </c>
@@ -5337,7 +5337,7 @@
       <c r="S20" s="135"/>
       <c r="T20" s="136"/>
     </row>
-    <row r="21" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="52">
         <v>10</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="124" t="s">
         <v>48</v>
       </c>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="T22" s="58"/>
     </row>
-    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="146"/>
       <c r="B23" s="121"/>
       <c r="C23" s="38"/>
@@ -5461,7 +5461,7 @@
       </c>
       <c r="T23" s="58"/>
     </row>
-    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="139"/>
       <c r="B24" s="121"/>
       <c r="C24" s="36"/>
@@ -5483,7 +5483,7 @@
       <c r="S24" s="36"/>
       <c r="T24" s="55"/>
     </row>
-    <row r="25" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="139"/>
       <c r="B25" s="121"/>
       <c r="C25" s="36"/>
@@ -5505,7 +5505,7 @@
       <c r="S25" s="36"/>
       <c r="T25" s="55"/>
     </row>
-    <row r="26" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A26" s="139"/>
       <c r="B26" s="121"/>
       <c r="C26" s="36"/>
@@ -5529,7 +5529,7 @@
       <c r="S26" s="36"/>
       <c r="T26" s="55"/>
     </row>
-    <row r="27" spans="1:20" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" ht="28" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="134"/>
       <c r="B27" s="135"/>
       <c r="C27" s="135"/>
@@ -5551,7 +5551,7 @@
       <c r="S27" s="135"/>
       <c r="T27" s="136"/>
     </row>
-    <row r="28" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="143" t="s">
         <v>26</v>
       </c>
@@ -5577,7 +5577,7 @@
       <c r="S28" s="135"/>
       <c r="T28" s="136"/>
     </row>
-    <row r="29" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="52">
         <v>10</v>
       </c>
@@ -5613,7 +5613,7 @@
       <c r="S29" s="176"/>
       <c r="T29" s="177"/>
     </row>
-    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="124" t="s">
         <v>30</v>
       </c>
@@ -5645,7 +5645,7 @@
       <c r="S30" s="172"/>
       <c r="T30" s="163"/>
     </row>
-    <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="139"/>
       <c r="B31" s="121"/>
       <c r="C31" s="172"/>
@@ -5667,7 +5667,7 @@
       <c r="S31" s="172"/>
       <c r="T31" s="163"/>
     </row>
-    <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="139"/>
       <c r="B32" s="121"/>
       <c r="C32" s="172"/>
@@ -5689,7 +5689,7 @@
       <c r="S32" s="172"/>
       <c r="T32" s="163"/>
     </row>
-    <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="139"/>
       <c r="B33" s="121"/>
       <c r="C33" s="172"/>
@@ -5711,7 +5711,7 @@
       <c r="S33" s="172"/>
       <c r="T33" s="163"/>
     </row>
-    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A34" s="139"/>
       <c r="B34" s="121"/>
       <c r="C34" s="174"/>
@@ -5735,7 +5735,7 @@
       <c r="S34" s="174"/>
       <c r="T34" s="165"/>
     </row>
-    <row r="35" spans="1:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="34.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A35" s="134"/>
       <c r="B35" s="135"/>
       <c r="C35" s="135"/>
@@ -5757,7 +5757,7 @@
       <c r="S35" s="135"/>
       <c r="T35" s="136"/>
     </row>
-    <row r="36" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="137" t="s">
         <v>31</v>
       </c>
@@ -5783,7 +5783,7 @@
       <c r="S36" s="135"/>
       <c r="T36" s="136"/>
     </row>
-    <row r="37" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="52">
         <v>10</v>
       </c>
@@ -5839,7 +5839,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A38" s="124" t="s">
         <v>38</v>
       </c>
@@ -5883,7 +5883,7 @@
       <c r="S38" s="69"/>
       <c r="T38" s="69"/>
     </row>
-    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="124" t="s">
         <v>43</v>
       </c>
@@ -5923,7 +5923,7 @@
       <c r="S39" s="69"/>
       <c r="T39" s="69"/>
     </row>
-    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="124" t="s">
         <v>44</v>
       </c>
@@ -5957,7 +5957,7 @@
       <c r="S40" s="69"/>
       <c r="T40" s="69"/>
     </row>
-    <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A41" s="124" t="s">
         <v>59</v>
       </c>
@@ -5991,7 +5991,7 @@
       <c r="S41" s="69"/>
       <c r="T41" s="69"/>
     </row>
-    <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="124"/>
       <c r="B42" s="121"/>
       <c r="C42" s="46"/>
@@ -6019,7 +6019,7 @@
       <c r="S42" s="69"/>
       <c r="T42" s="69"/>
     </row>
-    <row r="43" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="123"/>
       <c r="B43" s="121"/>
       <c r="C43" s="46"/>
@@ -6047,7 +6047,7 @@
       <c r="S43" s="46"/>
       <c r="T43" s="46"/>
     </row>
-    <row r="44" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="123"/>
       <c r="B44" s="121"/>
       <c r="C44" s="46"/>
@@ -6075,7 +6075,7 @@
       <c r="S44" s="46"/>
       <c r="T44" s="46"/>
     </row>
-    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A45" s="123"/>
       <c r="B45" s="121"/>
       <c r="C45" s="46"/>
@@ -6097,7 +6097,7 @@
       <c r="S45" s="46"/>
       <c r="T45" s="46"/>
     </row>
-    <row r="46" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A46" s="124" t="s">
         <v>16</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="184" t="s">
         <v>0</v>
       </c>
@@ -6156,7 +6156,7 @@
       <c r="G49" s="135"/>
       <c r="H49" s="135"/>
     </row>
-    <row r="50" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="185"/>
       <c r="B50" s="121"/>
       <c r="C50" s="98" t="s">
@@ -6174,7 +6174,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A51" s="182" t="s">
         <v>5</v>
       </c>
@@ -6192,7 +6192,7 @@
       </c>
       <c r="H51" s="97"/>
     </row>
-    <row r="52" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A52" s="182" t="s">
         <v>31</v>
       </c>
@@ -6211,7 +6211,7 @@
       </c>
       <c r="H52" s="97"/>
     </row>
-    <row r="53" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:8" ht="15.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A53" s="182" t="s">
         <v>9</v>
       </c>
@@ -6498,28 +6498,28 @@
       <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.31640625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+    <col min="8" max="8" width="10.81640625" customWidth="1"/>
     <col min="9" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="7.5" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="7.6796875" customWidth="1"/>
+    <col min="15" max="15" width="7.31640625" customWidth="1"/>
     <col min="16" max="16" width="7.5" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" customWidth="1"/>
+    <col min="18" max="18" width="15.1796875" customWidth="1"/>
+    <col min="19" max="19" width="5.6796875" customWidth="1"/>
+    <col min="20" max="20" width="8.31640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="157" t="s">
         <v>0</v>
       </c>
@@ -6545,7 +6545,7 @@
       <c r="S1" s="160"/>
       <c r="T1" s="161"/>
     </row>
-    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="166"/>
       <c r="B2" s="121"/>
       <c r="C2" s="96" t="s">
@@ -6575,7 +6575,7 @@
       <c r="S2" s="162"/>
       <c r="T2" s="163"/>
     </row>
-    <row r="3" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="168" t="s">
         <v>5</v>
       </c>
@@ -6610,7 +6610,7 @@
       <c r="S3" s="162"/>
       <c r="T3" s="163"/>
     </row>
-    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="168" t="s">
         <v>7</v>
       </c>
@@ -6647,7 +6647,7 @@
       <c r="S4" s="162"/>
       <c r="T4" s="163"/>
     </row>
-    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="168" t="s">
         <v>9</v>
       </c>
@@ -6683,7 +6683,7 @@
       <c r="S5" s="164"/>
       <c r="T5" s="165"/>
     </row>
-    <row r="6" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="1">
       <c r="A6" s="154"/>
       <c r="B6" s="135"/>
       <c r="C6" s="135"/>
@@ -6705,7 +6705,7 @@
       <c r="S6" s="135"/>
       <c r="T6" s="136"/>
     </row>
-    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="143" t="s">
         <v>11</v>
       </c>
@@ -6731,7 +6731,7 @@
       <c r="S7" s="135"/>
       <c r="T7" s="136"/>
     </row>
-    <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="155">
         <v>17</v>
       </c>
@@ -6787,7 +6787,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="124" t="s">
         <v>64</v>
       </c>
@@ -6835,7 +6835,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="124" t="s">
         <v>40</v>
       </c>
@@ -6881,7 +6881,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="124" t="s">
         <v>38</v>
       </c>
@@ -6921,7 +6921,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="124" t="s">
         <v>45</v>
       </c>
@@ -6955,7 +6955,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="124" t="s">
         <v>66</v>
       </c>
@@ -6989,7 +6989,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="124" t="s">
         <v>67</v>
       </c>
@@ -7017,7 +7017,7 @@
       <c r="S14" s="36"/>
       <c r="T14" s="82"/>
     </row>
-    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="139"/>
       <c r="B15" s="121"/>
       <c r="C15" s="38"/>
@@ -7039,7 +7039,7 @@
       <c r="S15" s="36"/>
       <c r="T15" s="82"/>
     </row>
-    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="124" t="s">
         <v>16</v>
       </c>
@@ -7087,7 +7087,7 @@
       </c>
       <c r="U16" s="92"/>
     </row>
-    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="150"/>
       <c r="B17" s="135"/>
       <c r="C17" s="135"/>
@@ -7114,7 +7114,7 @@
         <v>37.64</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="47" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="47" customHeight="1" x14ac:dyDescent="1">
       <c r="A18" s="147" t="s">
         <v>18</v>
       </c>
@@ -7140,7 +7140,7 @@
       <c r="S18" s="135"/>
       <c r="T18" s="136"/>
     </row>
-    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="52">
         <v>17</v>
       </c>
@@ -7196,7 +7196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="145" t="s">
         <v>22</v>
       </c>
@@ -7228,7 +7228,7 @@
       <c r="S20" s="38"/>
       <c r="T20" s="85"/>
     </row>
-    <row r="21" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="149"/>
       <c r="B21" s="121"/>
       <c r="C21" s="38"/>
@@ -7250,7 +7250,7 @@
       <c r="S21" s="33"/>
       <c r="T21" s="57"/>
     </row>
-    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="139"/>
       <c r="B22" s="121"/>
       <c r="C22" s="36"/>
@@ -7272,7 +7272,7 @@
       <c r="S22" s="33"/>
       <c r="T22" s="57"/>
     </row>
-    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="139"/>
       <c r="B23" s="121"/>
       <c r="C23" s="36"/>
@@ -7294,7 +7294,7 @@
       <c r="S23" s="33"/>
       <c r="T23" s="57"/>
     </row>
-    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="139"/>
       <c r="B24" s="121"/>
       <c r="C24" s="36"/>
@@ -7316,7 +7316,7 @@
       <c r="S24" s="33"/>
       <c r="T24" s="57"/>
     </row>
-    <row r="25" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="134"/>
       <c r="B25" s="135"/>
       <c r="C25" s="135"/>
@@ -7338,7 +7338,7 @@
       <c r="S25" s="135"/>
       <c r="T25" s="136"/>
     </row>
-    <row r="26" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="1">
       <c r="A26" s="147" t="s">
         <v>23</v>
       </c>
@@ -7364,7 +7364,7 @@
       <c r="S26" s="135"/>
       <c r="T26" s="136"/>
     </row>
-    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="52">
         <v>17</v>
       </c>
@@ -7420,7 +7420,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="124" t="s">
         <v>68</v>
       </c>
@@ -7458,7 +7458,7 @@
       <c r="S28" s="38"/>
       <c r="T28" s="85"/>
     </row>
-    <row r="29" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="146"/>
       <c r="B29" s="121"/>
       <c r="C29" s="38"/>
@@ -7484,7 +7484,7 @@
       <c r="S29" s="38"/>
       <c r="T29" s="55"/>
     </row>
-    <row r="30" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="139"/>
       <c r="B30" s="121"/>
       <c r="C30" s="36"/>
@@ -7506,7 +7506,7 @@
       <c r="S30" s="36"/>
       <c r="T30" s="55"/>
     </row>
-    <row r="31" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="139"/>
       <c r="B31" s="121"/>
       <c r="C31" s="36"/>
@@ -7528,7 +7528,7 @@
       <c r="S31" s="36"/>
       <c r="T31" s="55"/>
     </row>
-    <row r="32" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="139"/>
       <c r="B32" s="121"/>
       <c r="C32" s="36"/>
@@ -7550,7 +7550,7 @@
       <c r="S32" s="36"/>
       <c r="T32" s="55"/>
     </row>
-    <row r="33" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="134"/>
       <c r="B33" s="135"/>
       <c r="C33" s="135"/>
@@ -7572,7 +7572,7 @@
       <c r="S33" s="135"/>
       <c r="T33" s="136"/>
     </row>
-    <row r="34" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A34" s="143" t="s">
         <v>26</v>
       </c>
@@ -7598,7 +7598,7 @@
       <c r="S34" s="135"/>
       <c r="T34" s="136"/>
     </row>
-    <row r="35" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A35" s="52">
         <v>17</v>
       </c>
@@ -7654,7 +7654,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="145" t="s">
         <v>30</v>
       </c>
@@ -7686,7 +7686,7 @@
       <c r="S36" s="69"/>
       <c r="T36" s="83"/>
     </row>
-    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="139"/>
       <c r="B37" s="121"/>
       <c r="C37" s="69"/>
@@ -7708,7 +7708,7 @@
       <c r="S37" s="69"/>
       <c r="T37" s="83"/>
     </row>
-    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A38" s="139"/>
       <c r="B38" s="121"/>
       <c r="C38" s="69"/>
@@ -7730,7 +7730,7 @@
       <c r="S38" s="69"/>
       <c r="T38" s="83"/>
     </row>
-    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="139"/>
       <c r="B39" s="121"/>
       <c r="C39" s="69"/>
@@ -7752,7 +7752,7 @@
       <c r="S39" s="69"/>
       <c r="T39" s="83"/>
     </row>
-    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="139"/>
       <c r="B40" s="121"/>
       <c r="C40" s="69"/>
@@ -7774,7 +7774,7 @@
       <c r="S40" s="69"/>
       <c r="T40" s="83"/>
     </row>
-    <row r="41" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A41" s="134"/>
       <c r="B41" s="135"/>
       <c r="C41" s="135"/>
@@ -7796,7 +7796,7 @@
       <c r="S41" s="135"/>
       <c r="T41" s="136"/>
     </row>
-    <row r="42" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="137" t="s">
         <v>31</v>
       </c>
@@ -7822,7 +7822,7 @@
       <c r="S42" s="135"/>
       <c r="T42" s="136"/>
     </row>
-    <row r="43" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="87">
         <v>17</v>
       </c>
@@ -7878,7 +7878,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="132" t="s">
         <v>34</v>
       </c>
@@ -7918,7 +7918,7 @@
       <c r="S44" s="38"/>
       <c r="T44" s="85"/>
     </row>
-    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A45" s="123"/>
       <c r="B45" s="121"/>
       <c r="C45" s="51"/>
@@ -7946,7 +7946,7 @@
       <c r="S45" s="69"/>
       <c r="T45" s="83"/>
     </row>
-    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A46" s="123"/>
       <c r="B46" s="121"/>
       <c r="C46" s="51"/>
@@ -7974,7 +7974,7 @@
       <c r="S46" s="69"/>
       <c r="T46" s="83"/>
     </row>
-    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="123"/>
       <c r="B47" s="121"/>
       <c r="C47" s="51"/>
@@ -8002,7 +8002,7 @@
       <c r="S47" s="69"/>
       <c r="T47" s="83"/>
     </row>
-    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A48" s="124"/>
       <c r="B48" s="121"/>
       <c r="C48" s="73"/>
@@ -8024,7 +8024,7 @@
       <c r="S48" s="69"/>
       <c r="T48" s="83"/>
     </row>
-    <row r="49" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="123"/>
       <c r="B49" s="121"/>
       <c r="C49" s="73"/>
@@ -8046,7 +8046,7 @@
       <c r="S49" s="46"/>
       <c r="T49" s="68"/>
     </row>
-    <row r="50" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="123"/>
       <c r="B50" s="121"/>
       <c r="C50" s="73"/>
@@ -8068,7 +8068,7 @@
       <c r="S50" s="46"/>
       <c r="T50" s="68"/>
     </row>
-    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A51" s="123"/>
       <c r="B51" s="121"/>
       <c r="C51" s="73"/>
@@ -8090,7 +8090,7 @@
       <c r="S51" s="46"/>
       <c r="T51" s="68"/>
     </row>
-    <row r="52" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A52" s="122" t="s">
         <v>16</v>
       </c>
@@ -8137,7 +8137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A53" s="128"/>
       <c r="B53" s="129"/>
       <c r="C53" s="129"/>
@@ -8468,27 +8468,27 @@
       <selection activeCell="I10" sqref="I10:J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="6.83203125" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.1796875" customWidth="1"/>
+    <col min="3" max="3" width="6.81640625" customWidth="1"/>
+    <col min="4" max="4" width="11.31640625" customWidth="1"/>
     <col min="5" max="5" width="11.5" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.6796875" customWidth="1"/>
     <col min="7" max="7" width="6" customWidth="1"/>
     <col min="8" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="7.5" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" customWidth="1"/>
+    <col min="12" max="12" width="12.81640625" customWidth="1"/>
+    <col min="15" max="15" width="7.31640625" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
     <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="15.1640625" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.1796875" customWidth="1"/>
+    <col min="19" max="19" width="5.6796875" customWidth="1"/>
     <col min="20" max="20" width="11.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A1" s="157" t="s">
         <v>0</v>
       </c>
@@ -8514,7 +8514,7 @@
       <c r="S1" s="160"/>
       <c r="T1" s="161"/>
     </row>
-    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="166"/>
       <c r="B2" s="121"/>
       <c r="C2" s="96" t="s">
@@ -8544,7 +8544,7 @@
       <c r="S2" s="162"/>
       <c r="T2" s="163"/>
     </row>
-    <row r="3" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" ht="19" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A3" s="168" t="s">
         <v>5</v>
       </c>
@@ -8579,7 +8579,7 @@
       <c r="S3" s="162"/>
       <c r="T3" s="163"/>
     </row>
-    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A4" s="168" t="s">
         <v>7</v>
       </c>
@@ -8614,7 +8614,7 @@
       <c r="S4" s="162"/>
       <c r="T4" s="163"/>
     </row>
-    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:21" ht="20" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A5" s="168" t="s">
         <v>9</v>
       </c>
@@ -8651,7 +8651,7 @@
       <c r="S5" s="164"/>
       <c r="T5" s="165"/>
     </row>
-    <row r="6" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" ht="27" customHeight="1" x14ac:dyDescent="1">
       <c r="A6" s="154"/>
       <c r="B6" s="135"/>
       <c r="C6" s="135"/>
@@ -8673,7 +8673,7 @@
       <c r="S6" s="135"/>
       <c r="T6" s="136"/>
     </row>
-    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:21" ht="45" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A7" s="143" t="s">
         <v>11</v>
       </c>
@@ -8699,7 +8699,7 @@
       <c r="S7" s="135"/>
       <c r="T7" s="136"/>
     </row>
-    <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A8" s="155">
         <v>24</v>
       </c>
@@ -8755,7 +8755,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A9" s="124" t="s">
         <v>48</v>
       </c>
@@ -8795,7 +8795,7 @@
       <c r="S9" s="38"/>
       <c r="T9" s="36"/>
     </row>
-    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A10" s="127" t="s">
         <v>56</v>
       </c>
@@ -8823,7 +8823,7 @@
       <c r="S10" s="38"/>
       <c r="T10" s="70"/>
     </row>
-    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A11" s="153"/>
       <c r="B11" s="121"/>
       <c r="C11" s="38"/>
@@ -8845,7 +8845,7 @@
       <c r="S11" s="38"/>
       <c r="T11" s="71"/>
     </row>
-    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A12" s="152"/>
       <c r="B12" s="121"/>
       <c r="C12" s="38"/>
@@ -8867,7 +8867,7 @@
       <c r="S12" s="38"/>
       <c r="T12" s="70"/>
     </row>
-    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A13" s="153"/>
       <c r="B13" s="121"/>
       <c r="C13" s="38"/>
@@ -8889,7 +8889,7 @@
       <c r="S13" s="38"/>
       <c r="T13" s="70"/>
     </row>
-    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A14" s="152"/>
       <c r="B14" s="121"/>
       <c r="C14" s="38"/>
@@ -8911,7 +8911,7 @@
       <c r="S14" s="38"/>
       <c r="T14" s="70"/>
     </row>
-    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="139"/>
       <c r="B15" s="121"/>
       <c r="C15" s="38"/>
@@ -8933,7 +8933,7 @@
       <c r="S15" s="38"/>
       <c r="T15" s="70"/>
     </row>
-    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:21" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A16" s="124" t="s">
         <v>16</v>
       </c>
@@ -8981,7 +8981,7 @@
       </c>
       <c r="U16" s="92"/>
     </row>
-    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A17" s="150"/>
       <c r="B17" s="135"/>
       <c r="C17" s="135"/>
@@ -9008,7 +9008,7 @@
         <v>7.1999999999999993</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="47" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" ht="47" customHeight="1" x14ac:dyDescent="1">
       <c r="A18" s="147" t="s">
         <v>18</v>
       </c>
@@ -9034,7 +9034,7 @@
       <c r="S18" s="135"/>
       <c r="T18" s="136"/>
     </row>
-    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A19" s="52">
         <v>24</v>
       </c>
@@ -9090,7 +9090,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A20" s="145" t="s">
         <v>22</v>
       </c>
@@ -9122,7 +9122,7 @@
       <c r="S20" s="38"/>
       <c r="T20" s="85"/>
     </row>
-    <row r="21" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="149"/>
       <c r="B21" s="121"/>
       <c r="C21" s="38"/>
@@ -9144,7 +9144,7 @@
       <c r="S21" s="33"/>
       <c r="T21" s="57"/>
     </row>
-    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="139"/>
       <c r="B22" s="121"/>
       <c r="C22" s="36"/>
@@ -9166,7 +9166,7 @@
       <c r="S22" s="33"/>
       <c r="T22" s="57"/>
     </row>
-    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A23" s="139"/>
       <c r="B23" s="121"/>
       <c r="C23" s="36"/>
@@ -9188,7 +9188,7 @@
       <c r="S23" s="33"/>
       <c r="T23" s="57"/>
     </row>
-    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A24" s="139"/>
       <c r="B24" s="121"/>
       <c r="C24" s="36"/>
@@ -9210,7 +9210,7 @@
       <c r="S24" s="33"/>
       <c r="T24" s="57"/>
     </row>
-    <row r="25" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A25" s="134"/>
       <c r="B25" s="135"/>
       <c r="C25" s="135"/>
@@ -9232,7 +9232,7 @@
       <c r="S25" s="135"/>
       <c r="T25" s="136"/>
     </row>
-    <row r="26" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="44" customHeight="1" x14ac:dyDescent="1">
       <c r="A26" s="147" t="s">
         <v>23</v>
       </c>
@@ -9258,7 +9258,7 @@
       <c r="S26" s="135"/>
       <c r="T26" s="136"/>
     </row>
-    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A27" s="52">
         <v>24</v>
       </c>
@@ -9314,7 +9314,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A28" s="148" t="s">
         <v>25</v>
       </c>
@@ -9350,7 +9350,7 @@
       <c r="S28" s="38"/>
       <c r="T28" s="38"/>
     </row>
-    <row r="29" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A29" s="146"/>
       <c r="B29" s="121"/>
       <c r="C29" s="38"/>
@@ -9372,7 +9372,7 @@
       <c r="S29" s="38"/>
       <c r="T29" s="55"/>
     </row>
-    <row r="30" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A30" s="139"/>
       <c r="B30" s="121"/>
       <c r="C30" s="36"/>
@@ -9394,7 +9394,7 @@
       <c r="S30" s="36"/>
       <c r="T30" s="55"/>
     </row>
-    <row r="31" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A31" s="139"/>
       <c r="B31" s="121"/>
       <c r="C31" s="36"/>
@@ -9416,7 +9416,7 @@
       <c r="S31" s="36"/>
       <c r="T31" s="55"/>
     </row>
-    <row r="32" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A32" s="139"/>
       <c r="B32" s="121"/>
       <c r="C32" s="36"/>
@@ -9438,7 +9438,7 @@
       <c r="S32" s="36"/>
       <c r="T32" s="55"/>
     </row>
-    <row r="33" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:20" ht="19" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A33" s="134"/>
       <c r="B33" s="135"/>
       <c r="C33" s="135"/>
@@ -9460,7 +9460,7 @@
       <c r="S33" s="135"/>
       <c r="T33" s="136"/>
     </row>
-    <row r="34" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:20" ht="23.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A34" s="143" t="s">
         <v>26</v>
       </c>
@@ -9486,7 +9486,7 @@
       <c r="S34" s="135"/>
       <c r="T34" s="136"/>
     </row>
-    <row r="35" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A35" s="52">
         <v>24</v>
       </c>
@@ -9542,7 +9542,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="145" t="s">
         <v>30</v>
       </c>
@@ -9574,7 +9574,7 @@
       <c r="S36" s="69"/>
       <c r="T36" s="83"/>
     </row>
-    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A37" s="139"/>
       <c r="B37" s="121"/>
       <c r="C37" s="69"/>
@@ -9596,7 +9596,7 @@
       <c r="S37" s="69"/>
       <c r="T37" s="83"/>
     </row>
-    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A38" s="139"/>
       <c r="B38" s="121"/>
       <c r="C38" s="69"/>
@@ -9618,7 +9618,7 @@
       <c r="S38" s="69"/>
       <c r="T38" s="83"/>
     </row>
-    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A39" s="139"/>
       <c r="B39" s="121"/>
       <c r="C39" s="69"/>
@@ -9640,7 +9640,7 @@
       <c r="S39" s="69"/>
       <c r="T39" s="83"/>
     </row>
-    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A40" s="139"/>
       <c r="B40" s="121"/>
       <c r="C40" s="69"/>
@@ -9662,7 +9662,7 @@
       <c r="S40" s="69"/>
       <c r="T40" s="83"/>
     </row>
-    <row r="41" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:20" ht="17" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A41" s="134"/>
       <c r="B41" s="135"/>
       <c r="C41" s="135"/>
@@ -9684,7 +9684,7 @@
       <c r="S41" s="135"/>
       <c r="T41" s="136"/>
     </row>
-    <row r="42" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:20" ht="43.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A42" s="137" t="s">
         <v>31</v>
       </c>
@@ -9710,7 +9710,7 @@
       <c r="S42" s="135"/>
       <c r="T42" s="136"/>
     </row>
-    <row r="43" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:20" ht="21" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A43" s="87">
         <v>24</v>
       </c>
@@ -9766,7 +9766,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A44" s="132" t="s">
         <v>34</v>
       </c>
@@ -9798,7 +9798,7 @@
       <c r="S44" s="38"/>
       <c r="T44" s="85"/>
     </row>
-    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A45" s="123"/>
       <c r="B45" s="121"/>
       <c r="C45" s="51"/>
@@ -9820,7 +9820,7 @@
       <c r="S45" s="69"/>
       <c r="T45" s="83"/>
     </row>
-    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A46" s="123"/>
       <c r="B46" s="121"/>
       <c r="C46" s="51"/>
@@ -9841,7 +9841,7 @@
       <c r="S46" s="69"/>
       <c r="T46" s="83"/>
     </row>
-    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A47" s="123"/>
       <c r="B47" s="121"/>
       <c r="C47" s="51"/>
@@ -9863,7 +9863,7 @@
       <c r="S47" s="69"/>
       <c r="T47" s="83"/>
     </row>
-    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A48" s="124"/>
       <c r="B48" s="121"/>
       <c r="C48" s="73"/>
@@ -9885,7 +9885,7 @@
       <c r="S48" s="69"/>
       <c r="T48" s="83"/>
     </row>
-    <row r="49" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:20" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A49" s="123"/>
       <c r="B49" s="121"/>
       <c r="C49" s="73"/>
@@ -9907,7 +9907,7 @@
       <c r="S49" s="46"/>
       <c r="T49" s="68"/>
     </row>
-    <row r="50" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:20" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A50" s="123"/>
       <c r="B50" s="121"/>
       <c r="C50" s="73"/>
@@ -9929,7 +9929,7 @@
       <c r="S50" s="46"/>
       <c r="T50" s="68"/>
     </row>
-    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A51" s="123"/>
       <c r="B51" s="121"/>
       <c r="C51" s="73"/>
@@ -9951,7 +9951,7 @@
       <c r="S51" s="46"/>
       <c r="T51" s="68"/>
     </row>
-    <row r="52" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A52" s="122" t="s">
         <v>16</v>
       </c>
@@ -9998,7 +9998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:20" ht="16.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A53" s="128"/>
       <c r="B53" s="129"/>
       <c r="C53" s="129"/>
@@ -10335,29 +10335,29 @@
       <selection activeCell="G48" sqref="G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="3" max="3" width="4.83203125" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" customWidth="1"/>
-    <col min="5" max="5" width="4.83203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" customWidth="1"/>
-    <col min="7" max="7" width="4.83203125" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="4.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="13.6796875" customWidth="1"/>
+    <col min="3" max="3" width="4.81640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6796875" customWidth="1"/>
+    <col min="5" max="5" width="4.81640625" customWidth="1"/>
+    <col min="6" max="6" width="13.6796875" customWidth="1"/>
+    <col min="7" max="7" width="4.81640625" customWidth="1"/>
+    <col min="8" max="8" width="13.6796875" customWidth="1"/>
+    <col min="9" max="9" width="4.81640625" customWidth="1"/>
+    <col min="10" max="10" width="13.6796875" customWidth="1"/>
     <col min="11" max="17" width="2.5" customWidth="1"/>
     <col min="18" max="18" width="1.5" customWidth="1"/>
     <col min="19" max="25" width="2.5" customWidth="1"/>
     <col min="26" max="26" width="1.5" customWidth="1"/>
     <col min="27" max="27" width="7.5" customWidth="1"/>
     <col min="28" max="28" width="6.5" customWidth="1"/>
-    <col min="29" max="29" width="17.1640625" customWidth="1"/>
-    <col min="30" max="30" width="10.33203125" customWidth="1"/>
+    <col min="29" max="29" width="17.1796875" customWidth="1"/>
+    <col min="30" max="30" width="10.31640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:32" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="207">
         <f>DATE(AD18,AD20,1)</f>
         <v>44562</v>
@@ -10392,7 +10392,7 @@
       <c r="X1" s="208"/>
       <c r="Y1" s="208"/>
     </row>
-    <row r="2" spans="1:32" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:32" s="3" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A2" s="208"/>
       <c r="B2" s="208"/>
       <c r="C2" s="208"/>
@@ -10460,7 +10460,7 @@
         <v>S</v>
       </c>
     </row>
-    <row r="3" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="209"/>
       <c r="B3" s="209"/>
       <c r="C3" s="209"/>
@@ -10533,7 +10533,7 @@
       <c r="AD3" s="3"/>
       <c r="AE3" s="3"/>
     </row>
-    <row r="4" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="209"/>
       <c r="B4" s="209"/>
       <c r="C4" s="209"/>
@@ -10606,7 +10606,7 @@
       <c r="AD4" s="3"/>
       <c r="AE4" s="3"/>
     </row>
-    <row r="5" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="209"/>
       <c r="B5" s="209"/>
       <c r="C5" s="209"/>
@@ -10679,7 +10679,7 @@
       <c r="AD5" s="3"/>
       <c r="AE5" s="3"/>
     </row>
-    <row r="6" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="209"/>
       <c r="B6" s="209"/>
       <c r="C6" s="209"/>
@@ -10752,7 +10752,7 @@
       <c r="AD6" s="3"/>
       <c r="AE6" s="3"/>
     </row>
-    <row r="7" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:32" s="4" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="209"/>
       <c r="B7" s="209"/>
       <c r="C7" s="209"/>
@@ -10825,7 +10825,7 @@
       <c r="AD7" s="3"/>
       <c r="AE7" s="3"/>
     </row>
-    <row r="8" spans="1:32" s="5" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:32" s="5" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -10895,7 +10895,7 @@
       </c>
       <c r="Z8" s="24"/>
     </row>
-    <row r="9" spans="1:32" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" s="1" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.8">
       <c r="A9" s="210">
         <f>A10</f>
         <v>44556</v>
@@ -10957,7 +10957,7 @@
       </c>
       <c r="AF9" s="31"/>
     </row>
-    <row r="10" spans="1:32" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A10" s="14">
         <f>$A$1-(WEEKDAY($A$1,1)-(start_day-1))-IF((WEEKDAY($A$1,1)-(start_day-1))&lt;=0,7,0)+1</f>
         <v>44556</v>
@@ -11019,7 +11019,7 @@
       </c>
       <c r="AF10" s="32"/>
     </row>
-    <row r="11" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A11" s="206"/>
       <c r="B11" s="195"/>
       <c r="C11" s="204"/>
@@ -11047,7 +11047,7 @@
       <c r="Y11" s="195"/>
       <c r="Z11" s="196"/>
     </row>
-    <row r="12" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A12" s="206"/>
       <c r="B12" s="195"/>
       <c r="C12" s="204"/>
@@ -11075,7 +11075,7 @@
       <c r="Y12" s="195"/>
       <c r="Z12" s="196"/>
     </row>
-    <row r="13" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A13" s="206"/>
       <c r="B13" s="195"/>
       <c r="C13" s="204"/>
@@ -11103,7 +11103,7 @@
       <c r="Y13" s="195"/>
       <c r="Z13" s="196"/>
     </row>
-    <row r="14" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A14" s="206"/>
       <c r="B14" s="195"/>
       <c r="C14" s="204"/>
@@ -11131,7 +11131,7 @@
       <c r="Y14" s="195"/>
       <c r="Z14" s="196"/>
     </row>
-    <row r="15" spans="1:32" s="2" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:32" s="2" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A15" s="205"/>
       <c r="B15" s="192"/>
       <c r="C15" s="203"/>
@@ -11160,7 +11160,7 @@
       <c r="Z15" s="193"/>
       <c r="AA15" s="1"/>
     </row>
-    <row r="16" spans="1:32" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A16" s="14">
         <f>S10+1</f>
         <v>44563</v>
@@ -11214,7 +11214,7 @@
       <c r="AC16" s="10"/>
       <c r="AD16" s="10"/>
     </row>
-    <row r="17" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A17" s="206"/>
       <c r="B17" s="195"/>
       <c r="C17" s="204"/>
@@ -11243,7 +11243,7 @@
       <c r="Z17" s="196"/>
       <c r="AB17" s="10"/>
     </row>
-    <row r="18" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A18" s="206"/>
       <c r="B18" s="195"/>
       <c r="C18" s="204"/>
@@ -11278,7 +11278,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="19" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A19" s="206"/>
       <c r="B19" s="195"/>
       <c r="C19" s="204"/>
@@ -11310,7 +11310,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A20" s="206"/>
       <c r="B20" s="195"/>
       <c r="C20" s="204"/>
@@ -11345,7 +11345,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:31" s="2" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:31" s="2" customFormat="1" ht="13.25" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A21" s="205"/>
       <c r="B21" s="192"/>
       <c r="C21" s="203"/>
@@ -11378,7 +11378,7 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:31" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A22" s="14">
         <f>S16+1</f>
         <v>44570</v>
@@ -11433,7 +11433,7 @@
       <c r="AD22" s="2"/>
       <c r="AE22" s="2"/>
     </row>
-    <row r="23" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A23" s="206"/>
       <c r="B23" s="195"/>
       <c r="C23" s="204"/>
@@ -11463,7 +11463,7 @@
       <c r="AC23" s="10"/>
       <c r="AD23" s="10"/>
     </row>
-    <row r="24" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A24" s="206"/>
       <c r="B24" s="195"/>
       <c r="C24" s="204"/>
@@ -11499,7 +11499,7 @@
       </c>
       <c r="AE24" s="2"/>
     </row>
-    <row r="25" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A25" s="206"/>
       <c r="B25" s="195"/>
       <c r="C25" s="204"/>
@@ -11530,7 +11530,7 @@
       <c r="AC25" s="10"/>
       <c r="AD25" s="10"/>
     </row>
-    <row r="26" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A26" s="206"/>
       <c r="B26" s="195"/>
       <c r="C26" s="204"/>
@@ -11559,7 +11559,7 @@
       <c r="Z26" s="196"/>
       <c r="AD26" s="10"/>
     </row>
-    <row r="27" spans="1:31" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A27" s="205"/>
       <c r="B27" s="192"/>
       <c r="C27" s="203"/>
@@ -11590,7 +11590,7 @@
       <c r="AD27" s="10"/>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A28" s="14">
         <f>S22+1</f>
         <v>44577</v>
@@ -11644,7 +11644,7 @@
       <c r="AC28" s="10"/>
       <c r="AD28" s="10"/>
     </row>
-    <row r="29" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A29" s="206"/>
       <c r="B29" s="195"/>
       <c r="C29" s="204"/>
@@ -11677,7 +11677,7 @@
       </c>
       <c r="AD29" s="10"/>
     </row>
-    <row r="30" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A30" s="206"/>
       <c r="B30" s="195"/>
       <c r="C30" s="204"/>
@@ -11711,7 +11711,7 @@
       <c r="AD30" s="10"/>
       <c r="AE30" s="2"/>
     </row>
-    <row r="31" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A31" s="206"/>
       <c r="B31" s="195"/>
       <c r="C31" s="204"/>
@@ -11741,7 +11741,7 @@
       <c r="AC31" s="10"/>
       <c r="AD31" s="10"/>
     </row>
-    <row r="32" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A32" s="206"/>
       <c r="B32" s="195"/>
       <c r="C32" s="204"/>
@@ -11770,7 +11770,7 @@
       <c r="Z32" s="196"/>
       <c r="AD32" s="10"/>
     </row>
-    <row r="33" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A33" s="205"/>
       <c r="B33" s="192"/>
       <c r="C33" s="203"/>
@@ -11801,7 +11801,7 @@
       <c r="AD33" s="1"/>
       <c r="AE33" s="1"/>
     </row>
-    <row r="34" spans="1:31" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" s="1" customFormat="1" ht="18.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A34" s="14">
         <f>S28+1</f>
         <v>44584</v>
@@ -11854,7 +11854,7 @@
       </c>
       <c r="AC34" s="10"/>
     </row>
-    <row r="35" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A35" s="206"/>
       <c r="B35" s="195"/>
       <c r="C35" s="204"/>
@@ -11886,7 +11886,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:31" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A36" s="206"/>
       <c r="B36" s="195"/>
       <c r="C36" s="204"/>
@@ -11917,7 +11917,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="37" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A37" s="206"/>
       <c r="B37" s="195"/>
       <c r="C37" s="204"/>
@@ -11945,7 +11945,7 @@
       <c r="Y37" s="195"/>
       <c r="Z37" s="196"/>
     </row>
-    <row r="38" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A38" s="206"/>
       <c r="B38" s="195"/>
       <c r="C38" s="204"/>
@@ -11973,7 +11973,7 @@
       <c r="Y38" s="195"/>
       <c r="Z38" s="196"/>
     </row>
-    <row r="39" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:31" s="2" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A39" s="205"/>
       <c r="B39" s="192"/>
       <c r="C39" s="203"/>
@@ -12002,7 +12002,7 @@
       <c r="Z39" s="193"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="1:31" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" ht="18.5" customHeight="1" x14ac:dyDescent="0.7">
       <c r="A40" s="14">
         <f>S34+1</f>
         <v>44591</v>
@@ -12038,7 +12038,7 @@
       <c r="Y40" s="17"/>
       <c r="Z40" s="9"/>
     </row>
-    <row r="41" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.6">
       <c r="A41" s="206"/>
       <c r="B41" s="162"/>
       <c r="C41" s="204"/>
@@ -12066,7 +12066,7 @@
       <c r="Y41" s="6"/>
       <c r="Z41" s="8"/>
     </row>
-    <row r="42" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.6">
       <c r="A42" s="206"/>
       <c r="B42" s="162"/>
       <c r="C42" s="204"/>
@@ -12094,7 +12094,7 @@
       <c r="Y42" s="6"/>
       <c r="Z42" s="7"/>
     </row>
-    <row r="43" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:31" x14ac:dyDescent="0.6">
       <c r="A43" s="206"/>
       <c r="B43" s="162"/>
       <c r="C43" s="204"/>
@@ -12122,7 +12122,7 @@
       <c r="Y43" s="6"/>
       <c r="Z43" s="7"/>
     </row>
-    <row r="44" spans="1:31" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.6">
       <c r="A44" s="206"/>
       <c r="B44" s="162"/>
       <c r="C44" s="204"/>
@@ -12152,7 +12152,7 @@
       <c r="Y44" s="162"/>
       <c r="Z44" s="196"/>
     </row>
-    <row r="45" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.6">
       <c r="A45" s="205"/>
       <c r="B45" s="192"/>
       <c r="C45" s="203"/>

</xml_diff>